<commit_message>
Added a welcome page in the Excel file
</commit_message>
<xml_diff>
--- a/1roundfr.xlsx
+++ b/1roundfr.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://correoiueedu-my.sharepoint.com/personal/emlaucho_correo_iue_edu_co/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1623" documentId="13_ncr:1_{A8384D9E-B3A4-42B0-B746-DEE88CC48681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4804F86-DA87-4427-8AA0-302AA38DBC56}"/>
+  <xr:revisionPtr revIDLastSave="1733" documentId="13_ncr:1_{A8384D9E-B3A4-42B0-B746-DEE88CC48681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78A9453F-1E6D-40A5-8931-5BF359469FF8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data Searching Tool" sheetId="3" r:id="rId1"/>
-    <sheet name="Data" sheetId="1" r:id="rId2"/>
-    <sheet name="Data Comparator Tool" sheetId="2" r:id="rId3"/>
+    <sheet name="Welcome" sheetId="4" r:id="rId1"/>
+    <sheet name="Data Searching Tool" sheetId="3" r:id="rId2"/>
+    <sheet name="Data" sheetId="1" r:id="rId3"/>
+    <sheet name="Data Comparator Tool" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="candidate">'Data Comparator Tool'!$C$4</definedName>
+    <definedName name="candidate">'Data Comparator Tool'!$D$4</definedName>
     <definedName name="candidate_list">Data!$A$2:$A$12</definedName>
     <definedName name="city_list">Data!$B$1:$DC$1</definedName>
-    <definedName name="city1">'Data Comparator Tool'!$E$4</definedName>
-    <definedName name="city2">'Data Comparator Tool'!$F$4</definedName>
+    <definedName name="city1">'Data Comparator Tool'!$F$4</definedName>
+    <definedName name="city2">'Data Comparator Tool'!$G$4</definedName>
     <definedName name="vote_list">Data!$B$2:$DC$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="138">
   <si>
     <t>Ain</t>
   </si>
@@ -456,12 +457,6 @@
     <t>Cells that highlight either the candidate or department selected</t>
   </si>
   <si>
-    <t>Source</t>
-  </si>
-  <si>
-    <t>https://www.data.gouv.fr/fr/datasets/election-presidentielle-des-10-et-24-avril-2022-resultats-du-1er-tour/</t>
-  </si>
-  <si>
     <t>Amount of votes</t>
   </si>
   <si>
@@ -477,12 +472,21 @@
   <si>
     <t>Compare Departments</t>
   </si>
+  <si>
+    <t>Welcome</t>
+  </si>
+  <si>
+    <t>You can head to each page individually by clicking onto any link:</t>
+  </si>
+  <si>
+    <t>Source:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -523,6 +527,31 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="72"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color theme="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="11">
@@ -731,7 +760,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -785,6 +814,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -793,18 +823,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -845,261 +863,36 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="252">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="228">
     <dxf>
       <font>
         <b/>
@@ -5042,29 +4835,29 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Data Comparator Tool'!$B$8:$B$9</c:f>
+              <c:f>'Data Comparator Tool'!$C$8:$C$9</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Paris</c:v>
+                  <c:v>Polynésie française</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Loire-Atlantique</c:v>
+                  <c:v>Lot-et-Garonne</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Data Comparator Tool'!$C$8:$C$9</c:f>
+              <c:f>'Data Comparator Tool'!$D$8:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>80373</c:v>
+                  <c:v>11797</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60072</c:v>
+                  <c:v>50288</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6156,6 +5949,68 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>165340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1371600</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>45181</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A19ABFB-7F74-F7E1-5BB3-163414B61AB0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="205740" y="531100"/>
+          <a:ext cx="1775460" cy="611361"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6163,13 +6018,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>220980</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>99060</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>220980</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
@@ -6199,13 +6054,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>556260</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>167640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -6223,7 +6078,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8519160" y="350520"/>
+          <a:off x="9128760" y="350520"/>
           <a:ext cx="3139440" cy="1554480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6302,13 +6157,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>746760</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
@@ -6326,7 +6181,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2628900" y="4175760"/>
+          <a:off x="3238500" y="4175760"/>
           <a:ext cx="6263640" cy="1554480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6439,242 +6294,304 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>172960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>52801</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7E91FFB-5446-40F2-BB1F-55B51D023992}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="175260" y="355840"/>
+          <a:ext cx="1775460" cy="611361"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3A0354B0-5D88-49C3-9525-8391A8AF5D31}" name="Table24" displayName="Table24" ref="D22:DF33" totalsRowShown="0" headerRowDxfId="251" headerRowBorderDxfId="250" tableBorderDxfId="249" totalsRowBorderDxfId="248">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3A0354B0-5D88-49C3-9525-8391A8AF5D31}" name="Table24" displayName="Table24" ref="D22:DF33" totalsRowShown="0" headerRowDxfId="227" headerRowBorderDxfId="226" tableBorderDxfId="225" totalsRowBorderDxfId="224">
   <autoFilter ref="D22:DF33" xr:uid="{3A0354B0-5D88-49C3-9525-8391A8AF5D31}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D23:DF33">
     <sortCondition descending="1" ref="D1:D24"/>
   </sortState>
   <tableColumns count="107">
-    <tableColumn id="1" xr3:uid="{F3DE74AA-A1C4-49DB-8A78-1AAE869CCDAF}" name="Candidate" dataDxfId="247"/>
-    <tableColumn id="2" xr3:uid="{BA171EB7-7E8E-48C2-B9DF-CB804A4EC370}" name="Ain" dataDxfId="246"/>
-    <tableColumn id="3" xr3:uid="{E7EC2642-B061-4AFE-B8D5-8F1184B6281D}" name="Aisne" dataDxfId="245"/>
-    <tableColumn id="4" xr3:uid="{CC0B351E-85A0-4A28-85DB-73E42900D931}" name="Allier" dataDxfId="244"/>
-    <tableColumn id="5" xr3:uid="{6C20AE03-7F08-46C5-A587-A1EF3FA64DB3}" name="Alpes-Maritimes" dataDxfId="243"/>
-    <tableColumn id="6" xr3:uid="{AD9CF595-8DCA-4689-ADB7-AED083F307B9}" name="Alpes-de-Haute-Provence" dataDxfId="242"/>
-    <tableColumn id="7" xr3:uid="{DA6E6CD5-9760-4B5F-9879-7A30B2BF2955}" name="Ardennes" dataDxfId="241"/>
-    <tableColumn id="8" xr3:uid="{227900A8-C408-4F5A-BCE2-6EACC6060144}" name="Ardèche" dataDxfId="240"/>
-    <tableColumn id="9" xr3:uid="{C609488D-96D6-4CDB-A59F-A2CD0C72AEAF}" name="Ariège" dataDxfId="239"/>
-    <tableColumn id="10" xr3:uid="{49F47406-98E7-42AC-95D3-F910FD915349}" name="Aube" dataDxfId="238"/>
-    <tableColumn id="11" xr3:uid="{0CC5BE7D-FA78-40C4-A3FD-07740239CF2A}" name="Aude" dataDxfId="237"/>
-    <tableColumn id="12" xr3:uid="{A27BCA72-D0D7-4237-9E07-4B5200E17282}" name="Aveyron" dataDxfId="236"/>
-    <tableColumn id="13" xr3:uid="{F3ECA5FD-8D9D-4CCA-9404-3D9538529A05}" name="Bas-Rhin" dataDxfId="235"/>
-    <tableColumn id="14" xr3:uid="{19060157-0678-4E80-BF4B-94B798426816}" name="Bouches-du-Rhône" dataDxfId="234"/>
-    <tableColumn id="15" xr3:uid="{3EAADD1A-255A-42FA-94E3-1FFDC899ED88}" name="Calvados" dataDxfId="233"/>
-    <tableColumn id="16" xr3:uid="{32C85D24-678B-4C0D-8EFC-AEEF59B9411C}" name="Cantal" dataDxfId="232"/>
-    <tableColumn id="17" xr3:uid="{F483BDAA-8F8E-48D4-A7BA-45D4A45E9A82}" name="Charente" dataDxfId="231"/>
-    <tableColumn id="18" xr3:uid="{2880E672-5E75-44DA-B6F8-C0880A058BC8}" name="Charente-Maritime" dataDxfId="230"/>
-    <tableColumn id="19" xr3:uid="{3F15D640-2658-4F0E-ABE0-6C1539B0A335}" name="Cher" dataDxfId="229"/>
-    <tableColumn id="20" xr3:uid="{2C34A846-639D-4D94-900F-616949AFACF3}" name="Corrèze" dataDxfId="228"/>
-    <tableColumn id="21" xr3:uid="{35B53B71-A7FC-42F1-A77A-2041D0EF0B61}" name="Corse-du-Sud" dataDxfId="227"/>
-    <tableColumn id="22" xr3:uid="{A6D1FBFA-ADF9-4604-86CE-57D90E24D788}" name="Creuse" dataDxfId="226"/>
-    <tableColumn id="23" xr3:uid="{1F0A4296-1800-476F-8C7B-92EBFDC0AF71}" name="Côte-d'Or" dataDxfId="225"/>
-    <tableColumn id="24" xr3:uid="{75332ECD-5F4D-4FE4-90E4-0DEC904276A0}" name="Côtes-d'Armor" dataDxfId="224"/>
-    <tableColumn id="25" xr3:uid="{03A817D8-0A5F-4735-91E0-610BF31720B0}" name="Deux-Sèvres" dataDxfId="223"/>
-    <tableColumn id="26" xr3:uid="{583005BF-3CFD-4F8E-95BD-27B5A8B4E9BB}" name="Dordogne" dataDxfId="222"/>
-    <tableColumn id="27" xr3:uid="{9C2A5B4A-8B1E-4B86-9BB3-F0BBEBE58385}" name="Doubs" dataDxfId="221"/>
-    <tableColumn id="28" xr3:uid="{F7C50C96-CB98-4167-8156-A6F276F8ED01}" name="Drôme" dataDxfId="220"/>
-    <tableColumn id="29" xr3:uid="{06D87A0D-AFB3-474D-A346-6C3ED5C09E01}" name="Essonne" dataDxfId="219"/>
-    <tableColumn id="30" xr3:uid="{98FD0D3D-BCA3-42D8-8A2C-561002A47694}" name="Eure" dataDxfId="218"/>
-    <tableColumn id="31" xr3:uid="{966D75C2-CCB9-4ED3-925C-8787110D8974}" name="Eure-et-Loir" dataDxfId="217"/>
-    <tableColumn id="32" xr3:uid="{EDA55F78-8EEB-41C1-9442-CDB3762F65D0}" name="Finistère" dataDxfId="216"/>
-    <tableColumn id="33" xr3:uid="{149F11B4-E844-4B7D-AFB9-784C0058279B}" name="Gard" dataDxfId="215"/>
-    <tableColumn id="34" xr3:uid="{EFCA43FD-774E-4D68-B7B3-992B158E5BF2}" name="Gers" dataDxfId="214"/>
-    <tableColumn id="35" xr3:uid="{2C484DE4-FDAE-4C53-B8DE-8D4E7F215F76}" name="Gironde" dataDxfId="213"/>
-    <tableColumn id="36" xr3:uid="{78DB5CEF-AF70-487E-A261-32FF5902D255}" name="Guadeloupe" dataDxfId="212"/>
-    <tableColumn id="37" xr3:uid="{E3D3203E-E72C-4E57-9AB6-1B0DFD3EB099}" name="Guyane" dataDxfId="211"/>
-    <tableColumn id="38" xr3:uid="{EAD72A97-20F5-4E6C-85C5-DDF1935061F5}" name="Haut-Rhin" dataDxfId="210"/>
-    <tableColumn id="39" xr3:uid="{C87336E3-1B41-41EE-9053-573B7A48B6C2}" name="Haute-Corse" dataDxfId="209"/>
-    <tableColumn id="40" xr3:uid="{B523851E-D4F9-4625-872A-347EC5DC2641}" name="Haute-Garonne" dataDxfId="208"/>
-    <tableColumn id="41" xr3:uid="{3C5130FB-9F2C-47C9-927F-D0ADBEEC626E}" name="Haute-Loire" dataDxfId="207"/>
-    <tableColumn id="42" xr3:uid="{CDE471CC-E552-4913-B2B3-D856D1EDCD6E}" name="Haute-Marne" dataDxfId="206"/>
-    <tableColumn id="43" xr3:uid="{CFFD5D1A-BD32-4007-B3C7-B2D0DA2D8811}" name="Haute-Savoie" dataDxfId="205"/>
-    <tableColumn id="44" xr3:uid="{CC4DE2CF-B177-43C7-BBC2-A603D55EF083}" name="Haute-Saône" dataDxfId="204"/>
-    <tableColumn id="45" xr3:uid="{103DF6FF-6A8B-425B-95E3-B317D90F1A14}" name="Haute-Vienne" dataDxfId="203"/>
-    <tableColumn id="46" xr3:uid="{A641849E-6052-44D6-87EA-E7ACFEDA14FC}" name="Hautes-Alpes" dataDxfId="202"/>
-    <tableColumn id="47" xr3:uid="{122806EB-B706-4099-9B9E-7439957E9D6B}" name="Hautes-Pyrénées" dataDxfId="201"/>
-    <tableColumn id="48" xr3:uid="{B6946548-41A3-4E74-A088-8DC04DD34DBF}" name="Hauts-de-Seine" dataDxfId="200"/>
-    <tableColumn id="49" xr3:uid="{2C3FB8BC-C2F4-4648-85C5-1C3A62D32F9F}" name="Hérault" dataDxfId="199"/>
-    <tableColumn id="50" xr3:uid="{122ED3D9-313F-4652-9494-B1AAB8D82906}" name="Ille-et-Vilaine" dataDxfId="198"/>
-    <tableColumn id="51" xr3:uid="{FC7B1BED-BFF8-4410-AB29-2CC7CC292266}" name="Indre" dataDxfId="197"/>
-    <tableColumn id="52" xr3:uid="{227E4905-C919-42AB-9C8F-5B25B8C5A319}" name="Indre-et-Loire" dataDxfId="196"/>
-    <tableColumn id="53" xr3:uid="{06BE3711-B183-4C0E-963C-46314391170C}" name="Isère" dataDxfId="195"/>
-    <tableColumn id="54" xr3:uid="{D8AF6021-3BF1-4656-AD2C-86894EFFF275}" name="Jura" dataDxfId="194"/>
-    <tableColumn id="55" xr3:uid="{3DA86B1D-4108-47D5-A95D-378D552F346D}" name="La Réunion" dataDxfId="193"/>
-    <tableColumn id="56" xr3:uid="{5900183D-EE1D-488E-9C01-C16A5390A333}" name="Landes" dataDxfId="192"/>
-    <tableColumn id="57" xr3:uid="{F068EC56-072F-44CF-B8ED-B29FFE52507B}" name="Loir-et-Cher" dataDxfId="191"/>
-    <tableColumn id="58" xr3:uid="{889EE94F-726E-4CDD-81AB-56C9A9849EEB}" name="Loire" dataDxfId="190"/>
-    <tableColumn id="59" xr3:uid="{B92DD265-B92A-46E6-A9C3-779245445875}" name="Loire-Atlantique" dataDxfId="189"/>
-    <tableColumn id="60" xr3:uid="{C2C44259-BA1F-4CD2-91F5-17FE467185B0}" name="Loiret" dataDxfId="188"/>
-    <tableColumn id="61" xr3:uid="{A60E9ACC-8B21-4A63-8D11-7A17EF5FA720}" name="Lot" dataDxfId="187"/>
-    <tableColumn id="62" xr3:uid="{ABDDD8FF-680D-4946-B920-22490D90F7D8}" name="Lot-et-Garonne" dataDxfId="186"/>
-    <tableColumn id="63" xr3:uid="{BB0581B0-D74F-4949-A752-F83D02ED0E43}" name="Lozère" dataDxfId="185"/>
-    <tableColumn id="64" xr3:uid="{EB871B41-4F9D-47E2-B036-B700A85D3DC3}" name="Maine-et-Loire" dataDxfId="184"/>
-    <tableColumn id="65" xr3:uid="{D27820E5-99B3-4892-A852-57B6EE1995D4}" name="Manche" dataDxfId="183"/>
-    <tableColumn id="66" xr3:uid="{DF9B0ABF-B49C-4755-937A-9D5B2DB8CA05}" name="Marne" dataDxfId="182"/>
-    <tableColumn id="67" xr3:uid="{25BAB532-BC90-4CC5-8354-64E370BB6E6E}" name="Martinique" dataDxfId="181"/>
-    <tableColumn id="68" xr3:uid="{78CBB8D9-2CB5-4215-AA6E-F04B0393F2FB}" name="Mayenne" dataDxfId="180"/>
-    <tableColumn id="69" xr3:uid="{D3DEB96D-4338-47B7-9EF9-0BC83E90CB4A}" name="Mayotte" dataDxfId="179"/>
-    <tableColumn id="70" xr3:uid="{4B656955-ABAA-4808-8006-AEDE3514F09D}" name="Meurthe-et-Moselle" dataDxfId="178"/>
-    <tableColumn id="71" xr3:uid="{0A714115-ED3A-4FEF-B544-093F0607DAA2}" name="Meuse" dataDxfId="177"/>
-    <tableColumn id="72" xr3:uid="{B9936AE5-CE83-4113-8EA5-69499A419E10}" name="Morbihan" dataDxfId="176"/>
-    <tableColumn id="73" xr3:uid="{4B8191AC-3710-497B-A3B3-270B68719CFC}" name="Moselle" dataDxfId="175"/>
-    <tableColumn id="74" xr3:uid="{D2BAEBE2-63E7-4694-BC1E-F6589CA809AA}" name="Nièvre" dataDxfId="174"/>
-    <tableColumn id="75" xr3:uid="{1BDA71D3-7EBF-4606-9DC4-1D75DA32A900}" name="Nord" dataDxfId="173"/>
-    <tableColumn id="76" xr3:uid="{7F596044-06A6-45C8-9967-40C2000C751B}" name="Nouvelle-Calédonie" dataDxfId="172"/>
-    <tableColumn id="77" xr3:uid="{F7629DFC-C662-4204-80F3-6996E0C6D150}" name="Oise" dataDxfId="171"/>
-    <tableColumn id="78" xr3:uid="{FFAF73F3-A37B-4A77-AE98-7DE8036E554B}" name="Orne" dataDxfId="170"/>
-    <tableColumn id="79" xr3:uid="{C191916D-F4A5-49B0-97E2-489A2B1496E3}" name="Paris" dataDxfId="169"/>
-    <tableColumn id="80" xr3:uid="{ED57F766-B4F6-475F-B1D5-6B3A6D8370E9}" name="Pas-de-Calais" dataDxfId="168"/>
-    <tableColumn id="81" xr3:uid="{FF6311EA-A3BF-45F8-85B3-75D02445E8CC}" name="Polynésie française" dataDxfId="167"/>
-    <tableColumn id="82" xr3:uid="{7031D819-ADEA-4C8A-8742-A2171D3683FA}" name="Puy-de-Dôme" dataDxfId="166"/>
-    <tableColumn id="83" xr3:uid="{82DC6DEA-BDE0-4DE8-BD51-A9E7DE86031B}" name="Pyrénées-Atlantiques" dataDxfId="165"/>
-    <tableColumn id="84" xr3:uid="{6A78F76F-0957-41F0-8743-E95C5C098828}" name="Pyrénées-Orientales" dataDxfId="164"/>
-    <tableColumn id="85" xr3:uid="{D8B1F739-FBBF-4CC6-99F5-EA573306C44E}" name="Rhône" dataDxfId="163"/>
-    <tableColumn id="86" xr3:uid="{E19E4AC1-1146-4A6D-950E-8E08F761C0CD}" name="Saint-Martin/Saint-Barthélemy" dataDxfId="162"/>
-    <tableColumn id="87" xr3:uid="{A504ED2C-D81C-4D80-84A4-D5B4132FB7A4}" name="Saint-Pierre-et-Miquelon" dataDxfId="161"/>
-    <tableColumn id="88" xr3:uid="{E5A727D2-9E21-44A4-B78F-232A5C9E47A1}" name="Sarthe" dataDxfId="160"/>
-    <tableColumn id="89" xr3:uid="{EC31DE7B-F0D0-49B4-8588-6238FD3590AB}" name="Savoie" dataDxfId="159"/>
-    <tableColumn id="90" xr3:uid="{3D63C02A-1A31-421F-BBFA-F9DCD0BE08AC}" name="Saône-et-Loire" dataDxfId="158"/>
-    <tableColumn id="91" xr3:uid="{8FA3801D-D113-4402-BD27-BA0D068D753B}" name="Seine-Maritime" dataDxfId="157"/>
-    <tableColumn id="92" xr3:uid="{98D54EE6-8D07-42D1-912C-BA7FEFA4B5D6}" name="Seine-Saint-Denis" dataDxfId="156"/>
-    <tableColumn id="93" xr3:uid="{CED04F05-16F4-462B-A280-0F96DC578A51}" name="Seine-et-Marne" dataDxfId="155"/>
-    <tableColumn id="94" xr3:uid="{86E11E53-7A56-4ED8-AB7A-247AE2FD6973}" name="Somme" dataDxfId="154"/>
-    <tableColumn id="95" xr3:uid="{3D7E6035-FA7E-4C48-81BE-D8DBCB5DFC63}" name="Tarn" dataDxfId="153"/>
-    <tableColumn id="96" xr3:uid="{F32F9333-877D-496E-91D9-1FEF4F885812}" name="Tarn-et-Garonne" dataDxfId="152"/>
-    <tableColumn id="97" xr3:uid="{AA3B310C-9060-42EE-84F9-0CEA2C079DE9}" name="Territoire de Belfort" dataDxfId="151"/>
-    <tableColumn id="98" xr3:uid="{83F164FA-226C-4E8F-B987-13AAD82664D0}" name="Val-d'Oise" dataDxfId="150"/>
-    <tableColumn id="99" xr3:uid="{A9DAA10F-E7AD-4626-9039-33308E6DF7DB}" name="Val-de-Marne" dataDxfId="149"/>
-    <tableColumn id="100" xr3:uid="{D15ED985-5B82-4054-994B-5723FA8A1BDD}" name="Var" dataDxfId="148"/>
-    <tableColumn id="101" xr3:uid="{B12EABC1-6DE8-4BCD-BF30-8D2F72F4735A}" name="Vaucluse" dataDxfId="147"/>
-    <tableColumn id="102" xr3:uid="{F43C8E04-CECE-4837-AC30-1CFBC2EE7210}" name="Vendée" dataDxfId="146"/>
-    <tableColumn id="103" xr3:uid="{77C799D5-E8EB-4546-A354-41E9867DBC0F}" name="Vienne" dataDxfId="145"/>
-    <tableColumn id="104" xr3:uid="{9E8FD912-3E8A-44F9-8CA3-0C9792C698D1}" name="Vosges" dataDxfId="144"/>
-    <tableColumn id="105" xr3:uid="{83FBC55A-8461-4742-A2C3-214D4690AD55}" name="Wallis et Futuna" dataDxfId="143"/>
-    <tableColumn id="106" xr3:uid="{C361EEC1-7397-4A1D-BF8D-0C94D8CA3DE0}" name="Yonne" dataDxfId="142"/>
-    <tableColumn id="107" xr3:uid="{01B7A7F7-BCBD-47C9-A9BC-4A2B2E7CC853}" name="Yvelines" dataDxfId="141"/>
+    <tableColumn id="1" xr3:uid="{F3DE74AA-A1C4-49DB-8A78-1AAE869CCDAF}" name="Candidate" dataDxfId="223"/>
+    <tableColumn id="2" xr3:uid="{BA171EB7-7E8E-48C2-B9DF-CB804A4EC370}" name="Ain" dataDxfId="222"/>
+    <tableColumn id="3" xr3:uid="{E7EC2642-B061-4AFE-B8D5-8F1184B6281D}" name="Aisne" dataDxfId="221"/>
+    <tableColumn id="4" xr3:uid="{CC0B351E-85A0-4A28-85DB-73E42900D931}" name="Allier" dataDxfId="220"/>
+    <tableColumn id="5" xr3:uid="{6C20AE03-7F08-46C5-A587-A1EF3FA64DB3}" name="Alpes-Maritimes" dataDxfId="219"/>
+    <tableColumn id="6" xr3:uid="{AD9CF595-8DCA-4689-ADB7-AED083F307B9}" name="Alpes-de-Haute-Provence" dataDxfId="218"/>
+    <tableColumn id="7" xr3:uid="{DA6E6CD5-9760-4B5F-9879-7A30B2BF2955}" name="Ardennes" dataDxfId="217"/>
+    <tableColumn id="8" xr3:uid="{227900A8-C408-4F5A-BCE2-6EACC6060144}" name="Ardèche" dataDxfId="216"/>
+    <tableColumn id="9" xr3:uid="{C609488D-96D6-4CDB-A59F-A2CD0C72AEAF}" name="Ariège" dataDxfId="215"/>
+    <tableColumn id="10" xr3:uid="{49F47406-98E7-42AC-95D3-F910FD915349}" name="Aube" dataDxfId="214"/>
+    <tableColumn id="11" xr3:uid="{0CC5BE7D-FA78-40C4-A3FD-07740239CF2A}" name="Aude" dataDxfId="213"/>
+    <tableColumn id="12" xr3:uid="{A27BCA72-D0D7-4237-9E07-4B5200E17282}" name="Aveyron" dataDxfId="212"/>
+    <tableColumn id="13" xr3:uid="{F3ECA5FD-8D9D-4CCA-9404-3D9538529A05}" name="Bas-Rhin" dataDxfId="211"/>
+    <tableColumn id="14" xr3:uid="{19060157-0678-4E80-BF4B-94B798426816}" name="Bouches-du-Rhône" dataDxfId="210"/>
+    <tableColumn id="15" xr3:uid="{3EAADD1A-255A-42FA-94E3-1FFDC899ED88}" name="Calvados" dataDxfId="209"/>
+    <tableColumn id="16" xr3:uid="{32C85D24-678B-4C0D-8EFC-AEEF59B9411C}" name="Cantal" dataDxfId="208"/>
+    <tableColumn id="17" xr3:uid="{F483BDAA-8F8E-48D4-A7BA-45D4A45E9A82}" name="Charente" dataDxfId="207"/>
+    <tableColumn id="18" xr3:uid="{2880E672-5E75-44DA-B6F8-C0880A058BC8}" name="Charente-Maritime" dataDxfId="206"/>
+    <tableColumn id="19" xr3:uid="{3F15D640-2658-4F0E-ABE0-6C1539B0A335}" name="Cher" dataDxfId="205"/>
+    <tableColumn id="20" xr3:uid="{2C34A846-639D-4D94-900F-616949AFACF3}" name="Corrèze" dataDxfId="204"/>
+    <tableColumn id="21" xr3:uid="{35B53B71-A7FC-42F1-A77A-2041D0EF0B61}" name="Corse-du-Sud" dataDxfId="203"/>
+    <tableColumn id="22" xr3:uid="{A6D1FBFA-ADF9-4604-86CE-57D90E24D788}" name="Creuse" dataDxfId="202"/>
+    <tableColumn id="23" xr3:uid="{1F0A4296-1800-476F-8C7B-92EBFDC0AF71}" name="Côte-d'Or" dataDxfId="201"/>
+    <tableColumn id="24" xr3:uid="{75332ECD-5F4D-4FE4-90E4-0DEC904276A0}" name="Côtes-d'Armor" dataDxfId="200"/>
+    <tableColumn id="25" xr3:uid="{03A817D8-0A5F-4735-91E0-610BF31720B0}" name="Deux-Sèvres" dataDxfId="199"/>
+    <tableColumn id="26" xr3:uid="{583005BF-3CFD-4F8E-95BD-27B5A8B4E9BB}" name="Dordogne" dataDxfId="198"/>
+    <tableColumn id="27" xr3:uid="{9C2A5B4A-8B1E-4B86-9BB3-F0BBEBE58385}" name="Doubs" dataDxfId="197"/>
+    <tableColumn id="28" xr3:uid="{F7C50C96-CB98-4167-8156-A6F276F8ED01}" name="Drôme" dataDxfId="196"/>
+    <tableColumn id="29" xr3:uid="{06D87A0D-AFB3-474D-A346-6C3ED5C09E01}" name="Essonne" dataDxfId="195"/>
+    <tableColumn id="30" xr3:uid="{98FD0D3D-BCA3-42D8-8A2C-561002A47694}" name="Eure" dataDxfId="194"/>
+    <tableColumn id="31" xr3:uid="{966D75C2-CCB9-4ED3-925C-8787110D8974}" name="Eure-et-Loir" dataDxfId="193"/>
+    <tableColumn id="32" xr3:uid="{EDA55F78-8EEB-41C1-9442-CDB3762F65D0}" name="Finistère" dataDxfId="192"/>
+    <tableColumn id="33" xr3:uid="{149F11B4-E844-4B7D-AFB9-784C0058279B}" name="Gard" dataDxfId="191"/>
+    <tableColumn id="34" xr3:uid="{EFCA43FD-774E-4D68-B7B3-992B158E5BF2}" name="Gers" dataDxfId="190"/>
+    <tableColumn id="35" xr3:uid="{2C484DE4-FDAE-4C53-B8DE-8D4E7F215F76}" name="Gironde" dataDxfId="189"/>
+    <tableColumn id="36" xr3:uid="{78DB5CEF-AF70-487E-A261-32FF5902D255}" name="Guadeloupe" dataDxfId="188"/>
+    <tableColumn id="37" xr3:uid="{E3D3203E-E72C-4E57-9AB6-1B0DFD3EB099}" name="Guyane" dataDxfId="187"/>
+    <tableColumn id="38" xr3:uid="{EAD72A97-20F5-4E6C-85C5-DDF1935061F5}" name="Haut-Rhin" dataDxfId="186"/>
+    <tableColumn id="39" xr3:uid="{C87336E3-1B41-41EE-9053-573B7A48B6C2}" name="Haute-Corse" dataDxfId="185"/>
+    <tableColumn id="40" xr3:uid="{B523851E-D4F9-4625-872A-347EC5DC2641}" name="Haute-Garonne" dataDxfId="184"/>
+    <tableColumn id="41" xr3:uid="{3C5130FB-9F2C-47C9-927F-D0ADBEEC626E}" name="Haute-Loire" dataDxfId="183"/>
+    <tableColumn id="42" xr3:uid="{CDE471CC-E552-4913-B2B3-D856D1EDCD6E}" name="Haute-Marne" dataDxfId="182"/>
+    <tableColumn id="43" xr3:uid="{CFFD5D1A-BD32-4007-B3C7-B2D0DA2D8811}" name="Haute-Savoie" dataDxfId="181"/>
+    <tableColumn id="44" xr3:uid="{CC4DE2CF-B177-43C7-BBC2-A603D55EF083}" name="Haute-Saône" dataDxfId="180"/>
+    <tableColumn id="45" xr3:uid="{103DF6FF-6A8B-425B-95E3-B317D90F1A14}" name="Haute-Vienne" dataDxfId="179"/>
+    <tableColumn id="46" xr3:uid="{A641849E-6052-44D6-87EA-E7ACFEDA14FC}" name="Hautes-Alpes" dataDxfId="178"/>
+    <tableColumn id="47" xr3:uid="{122806EB-B706-4099-9B9E-7439957E9D6B}" name="Hautes-Pyrénées" dataDxfId="177"/>
+    <tableColumn id="48" xr3:uid="{B6946548-41A3-4E74-A088-8DC04DD34DBF}" name="Hauts-de-Seine" dataDxfId="176"/>
+    <tableColumn id="49" xr3:uid="{2C3FB8BC-C2F4-4648-85C5-1C3A62D32F9F}" name="Hérault" dataDxfId="175"/>
+    <tableColumn id="50" xr3:uid="{122ED3D9-313F-4652-9494-B1AAB8D82906}" name="Ille-et-Vilaine" dataDxfId="174"/>
+    <tableColumn id="51" xr3:uid="{FC7B1BED-BFF8-4410-AB29-2CC7CC292266}" name="Indre" dataDxfId="173"/>
+    <tableColumn id="52" xr3:uid="{227E4905-C919-42AB-9C8F-5B25B8C5A319}" name="Indre-et-Loire" dataDxfId="172"/>
+    <tableColumn id="53" xr3:uid="{06BE3711-B183-4C0E-963C-46314391170C}" name="Isère" dataDxfId="171"/>
+    <tableColumn id="54" xr3:uid="{D8AF6021-3BF1-4656-AD2C-86894EFFF275}" name="Jura" dataDxfId="170"/>
+    <tableColumn id="55" xr3:uid="{3DA86B1D-4108-47D5-A95D-378D552F346D}" name="La Réunion" dataDxfId="169"/>
+    <tableColumn id="56" xr3:uid="{5900183D-EE1D-488E-9C01-C16A5390A333}" name="Landes" dataDxfId="168"/>
+    <tableColumn id="57" xr3:uid="{F068EC56-072F-44CF-B8ED-B29FFE52507B}" name="Loir-et-Cher" dataDxfId="167"/>
+    <tableColumn id="58" xr3:uid="{889EE94F-726E-4CDD-81AB-56C9A9849EEB}" name="Loire" dataDxfId="166"/>
+    <tableColumn id="59" xr3:uid="{B92DD265-B92A-46E6-A9C3-779245445875}" name="Loire-Atlantique" dataDxfId="165"/>
+    <tableColumn id="60" xr3:uid="{C2C44259-BA1F-4CD2-91F5-17FE467185B0}" name="Loiret" dataDxfId="164"/>
+    <tableColumn id="61" xr3:uid="{A60E9ACC-8B21-4A63-8D11-7A17EF5FA720}" name="Lot" dataDxfId="163"/>
+    <tableColumn id="62" xr3:uid="{ABDDD8FF-680D-4946-B920-22490D90F7D8}" name="Lot-et-Garonne" dataDxfId="162"/>
+    <tableColumn id="63" xr3:uid="{BB0581B0-D74F-4949-A752-F83D02ED0E43}" name="Lozère" dataDxfId="161"/>
+    <tableColumn id="64" xr3:uid="{EB871B41-4F9D-47E2-B036-B700A85D3DC3}" name="Maine-et-Loire" dataDxfId="160"/>
+    <tableColumn id="65" xr3:uid="{D27820E5-99B3-4892-A852-57B6EE1995D4}" name="Manche" dataDxfId="159"/>
+    <tableColumn id="66" xr3:uid="{DF9B0ABF-B49C-4755-937A-9D5B2DB8CA05}" name="Marne" dataDxfId="158"/>
+    <tableColumn id="67" xr3:uid="{25BAB532-BC90-4CC5-8354-64E370BB6E6E}" name="Martinique" dataDxfId="157"/>
+    <tableColumn id="68" xr3:uid="{78CBB8D9-2CB5-4215-AA6E-F04B0393F2FB}" name="Mayenne" dataDxfId="156"/>
+    <tableColumn id="69" xr3:uid="{D3DEB96D-4338-47B7-9EF9-0BC83E90CB4A}" name="Mayotte" dataDxfId="155"/>
+    <tableColumn id="70" xr3:uid="{4B656955-ABAA-4808-8006-AEDE3514F09D}" name="Meurthe-et-Moselle" dataDxfId="154"/>
+    <tableColumn id="71" xr3:uid="{0A714115-ED3A-4FEF-B544-093F0607DAA2}" name="Meuse" dataDxfId="153"/>
+    <tableColumn id="72" xr3:uid="{B9936AE5-CE83-4113-8EA5-69499A419E10}" name="Morbihan" dataDxfId="152"/>
+    <tableColumn id="73" xr3:uid="{4B8191AC-3710-497B-A3B3-270B68719CFC}" name="Moselle" dataDxfId="151"/>
+    <tableColumn id="74" xr3:uid="{D2BAEBE2-63E7-4694-BC1E-F6589CA809AA}" name="Nièvre" dataDxfId="150"/>
+    <tableColumn id="75" xr3:uid="{1BDA71D3-7EBF-4606-9DC4-1D75DA32A900}" name="Nord" dataDxfId="149"/>
+    <tableColumn id="76" xr3:uid="{7F596044-06A6-45C8-9967-40C2000C751B}" name="Nouvelle-Calédonie" dataDxfId="148"/>
+    <tableColumn id="77" xr3:uid="{F7629DFC-C662-4204-80F3-6996E0C6D150}" name="Oise" dataDxfId="147"/>
+    <tableColumn id="78" xr3:uid="{FFAF73F3-A37B-4A77-AE98-7DE8036E554B}" name="Orne" dataDxfId="146"/>
+    <tableColumn id="79" xr3:uid="{C191916D-F4A5-49B0-97E2-489A2B1496E3}" name="Paris" dataDxfId="145"/>
+    <tableColumn id="80" xr3:uid="{ED57F766-B4F6-475F-B1D5-6B3A6D8370E9}" name="Pas-de-Calais" dataDxfId="144"/>
+    <tableColumn id="81" xr3:uid="{FF6311EA-A3BF-45F8-85B3-75D02445E8CC}" name="Polynésie française" dataDxfId="143"/>
+    <tableColumn id="82" xr3:uid="{7031D819-ADEA-4C8A-8742-A2171D3683FA}" name="Puy-de-Dôme" dataDxfId="142"/>
+    <tableColumn id="83" xr3:uid="{82DC6DEA-BDE0-4DE8-BD51-A9E7DE86031B}" name="Pyrénées-Atlantiques" dataDxfId="141"/>
+    <tableColumn id="84" xr3:uid="{6A78F76F-0957-41F0-8743-E95C5C098828}" name="Pyrénées-Orientales" dataDxfId="140"/>
+    <tableColumn id="85" xr3:uid="{D8B1F739-FBBF-4CC6-99F5-EA573306C44E}" name="Rhône" dataDxfId="139"/>
+    <tableColumn id="86" xr3:uid="{E19E4AC1-1146-4A6D-950E-8E08F761C0CD}" name="Saint-Martin/Saint-Barthélemy" dataDxfId="138"/>
+    <tableColumn id="87" xr3:uid="{A504ED2C-D81C-4D80-84A4-D5B4132FB7A4}" name="Saint-Pierre-et-Miquelon" dataDxfId="137"/>
+    <tableColumn id="88" xr3:uid="{E5A727D2-9E21-44A4-B78F-232A5C9E47A1}" name="Sarthe" dataDxfId="136"/>
+    <tableColumn id="89" xr3:uid="{EC31DE7B-F0D0-49B4-8588-6238FD3590AB}" name="Savoie" dataDxfId="135"/>
+    <tableColumn id="90" xr3:uid="{3D63C02A-1A31-421F-BBFA-F9DCD0BE08AC}" name="Saône-et-Loire" dataDxfId="134"/>
+    <tableColumn id="91" xr3:uid="{8FA3801D-D113-4402-BD27-BA0D068D753B}" name="Seine-Maritime" dataDxfId="133"/>
+    <tableColumn id="92" xr3:uid="{98D54EE6-8D07-42D1-912C-BA7FEFA4B5D6}" name="Seine-Saint-Denis" dataDxfId="132"/>
+    <tableColumn id="93" xr3:uid="{CED04F05-16F4-462B-A280-0F96DC578A51}" name="Seine-et-Marne" dataDxfId="131"/>
+    <tableColumn id="94" xr3:uid="{86E11E53-7A56-4ED8-AB7A-247AE2FD6973}" name="Somme" dataDxfId="130"/>
+    <tableColumn id="95" xr3:uid="{3D7E6035-FA7E-4C48-81BE-D8DBCB5DFC63}" name="Tarn" dataDxfId="129"/>
+    <tableColumn id="96" xr3:uid="{F32F9333-877D-496E-91D9-1FEF4F885812}" name="Tarn-et-Garonne" dataDxfId="128"/>
+    <tableColumn id="97" xr3:uid="{AA3B310C-9060-42EE-84F9-0CEA2C079DE9}" name="Territoire de Belfort" dataDxfId="127"/>
+    <tableColumn id="98" xr3:uid="{83F164FA-226C-4E8F-B987-13AAD82664D0}" name="Val-d'Oise" dataDxfId="126"/>
+    <tableColumn id="99" xr3:uid="{A9DAA10F-E7AD-4626-9039-33308E6DF7DB}" name="Val-de-Marne" dataDxfId="125"/>
+    <tableColumn id="100" xr3:uid="{D15ED985-5B82-4054-994B-5723FA8A1BDD}" name="Var" dataDxfId="124"/>
+    <tableColumn id="101" xr3:uid="{B12EABC1-6DE8-4BCD-BF30-8D2F72F4735A}" name="Vaucluse" dataDxfId="123"/>
+    <tableColumn id="102" xr3:uid="{F43C8E04-CECE-4837-AC30-1CFBC2EE7210}" name="Vendée" dataDxfId="122"/>
+    <tableColumn id="103" xr3:uid="{77C799D5-E8EB-4546-A354-41E9867DBC0F}" name="Vienne" dataDxfId="121"/>
+    <tableColumn id="104" xr3:uid="{9E8FD912-3E8A-44F9-8CA3-0C9792C698D1}" name="Vosges" dataDxfId="120"/>
+    <tableColumn id="105" xr3:uid="{83FBC55A-8461-4742-A2C3-214D4690AD55}" name="Wallis et Futuna" dataDxfId="119"/>
+    <tableColumn id="106" xr3:uid="{C361EEC1-7397-4A1D-BF8D-0C94D8CA3DE0}" name="Yonne" dataDxfId="118"/>
+    <tableColumn id="107" xr3:uid="{01B7A7F7-BCBD-47C9-A9BC-4A2B2E7CC853}" name="Yvelines" dataDxfId="117"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B7C971C4-144D-48D1-B8FF-303AF3E9CC5A}" name="Table2" displayName="Table2" ref="A1:DC12" totalsRowShown="0" headerRowDxfId="140" headerRowBorderDxfId="139" tableBorderDxfId="138" totalsRowBorderDxfId="137">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B7C971C4-144D-48D1-B8FF-303AF3E9CC5A}" name="Table2" displayName="Table2" ref="A1:DC12" totalsRowShown="0" headerRowDxfId="116" headerRowBorderDxfId="115" tableBorderDxfId="114" totalsRowBorderDxfId="113">
   <autoFilter ref="A1:DC12" xr:uid="{B7C971C4-144D-48D1-B8FF-303AF3E9CC5A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:DC12">
     <sortCondition descending="1" ref="A1:A12"/>
   </sortState>
   <tableColumns count="107">
-    <tableColumn id="1" xr3:uid="{27C8E1A7-4DD3-497E-9BB7-9E0EE471B6E9}" name="Candidate" dataDxfId="136"/>
-    <tableColumn id="2" xr3:uid="{8CCB92DA-03BE-4E04-9048-217E624457FE}" name="Ain" dataDxfId="135"/>
-    <tableColumn id="3" xr3:uid="{5850EA8D-19C4-464A-803C-AE76ED004BD3}" name="Aisne" dataDxfId="134"/>
-    <tableColumn id="4" xr3:uid="{A6D7EBC4-3FE3-4221-8CCA-78E0740E2B64}" name="Allier" dataDxfId="133"/>
-    <tableColumn id="5" xr3:uid="{BE876166-4E7F-40FA-968C-02CBE720939A}" name="Alpes-Maritimes" dataDxfId="132"/>
-    <tableColumn id="6" xr3:uid="{232532A6-0C44-4E86-A5AF-A317ECD29C04}" name="Alpes-de-Haute-Provence" dataDxfId="131"/>
-    <tableColumn id="7" xr3:uid="{2373349C-D894-424D-AA87-AEE39F79AD05}" name="Ardennes" dataDxfId="130"/>
-    <tableColumn id="8" xr3:uid="{2B73B324-EE11-4018-9BF9-84682AC1F105}" name="Ardèche" dataDxfId="129"/>
-    <tableColumn id="9" xr3:uid="{16372E34-A8F2-4A61-8F28-063FA267BC65}" name="Ariège" dataDxfId="128"/>
-    <tableColumn id="10" xr3:uid="{682605AC-2360-4778-9C99-8D2E17716ED5}" name="Aube" dataDxfId="127"/>
-    <tableColumn id="11" xr3:uid="{981C5C21-7AC7-47EA-A861-ADA53019D2EE}" name="Aude" dataDxfId="126"/>
-    <tableColumn id="12" xr3:uid="{8048A4F9-B569-4139-A8EF-B7CD7DC9AB56}" name="Aveyron" dataDxfId="125"/>
-    <tableColumn id="13" xr3:uid="{CAF3796D-7307-4506-8316-970783B565DE}" name="Bas-Rhin" dataDxfId="124"/>
-    <tableColumn id="14" xr3:uid="{92A27818-DB05-44C6-BDD3-489379907650}" name="Bouches-du-Rhône" dataDxfId="123"/>
-    <tableColumn id="15" xr3:uid="{09D411A4-73D7-4592-8926-BEBAF46A4E4F}" name="Calvados" dataDxfId="122"/>
-    <tableColumn id="16" xr3:uid="{3F66DE9E-989E-4D21-B8FE-5AB647243D04}" name="Cantal" dataDxfId="121"/>
-    <tableColumn id="17" xr3:uid="{A7691DC8-030B-4E6F-B599-4D694CC66BC2}" name="Charente" dataDxfId="120"/>
-    <tableColumn id="18" xr3:uid="{4312157F-5109-415F-BF4F-A5D40DCEF34A}" name="Charente-Maritime" dataDxfId="119"/>
-    <tableColumn id="19" xr3:uid="{1335A6BC-A79F-4F25-937E-7411352074B7}" name="Cher" dataDxfId="118"/>
-    <tableColumn id="20" xr3:uid="{ABB30B80-C652-4182-A93D-AE336859C19F}" name="Corrèze" dataDxfId="117"/>
-    <tableColumn id="21" xr3:uid="{150B3246-C696-4D43-BC4C-053D447C0C48}" name="Corse-du-Sud" dataDxfId="116"/>
-    <tableColumn id="22" xr3:uid="{61704F7C-FB36-4160-90D1-9181EB7D489E}" name="Creuse" dataDxfId="115"/>
-    <tableColumn id="23" xr3:uid="{BBC4F1BA-8753-4F7E-9BFA-E8F4E262C658}" name="Côte-d'Or" dataDxfId="114"/>
-    <tableColumn id="24" xr3:uid="{25DB42A6-CECF-429D-B06D-C4428313548B}" name="Côtes-d'Armor" dataDxfId="113"/>
-    <tableColumn id="25" xr3:uid="{78B8BED2-E7C2-402C-A723-5EEE3BB04CDC}" name="Deux-Sèvres" dataDxfId="112"/>
-    <tableColumn id="26" xr3:uid="{56BEE575-2617-400C-A0AE-FB05670ACE71}" name="Dordogne" dataDxfId="111"/>
-    <tableColumn id="27" xr3:uid="{5425430B-1026-4534-A351-16430171312D}" name="Doubs" dataDxfId="110"/>
-    <tableColumn id="28" xr3:uid="{FDD5121D-C879-457B-A2DF-C83B7CC13CD0}" name="Drôme" dataDxfId="109"/>
-    <tableColumn id="29" xr3:uid="{7B72C5EC-FFEA-4EE7-9221-9450CC387071}" name="Essonne" dataDxfId="108"/>
-    <tableColumn id="30" xr3:uid="{9F6C6700-5FAB-454E-B2D8-4065D439F10E}" name="Eure" dataDxfId="107"/>
-    <tableColumn id="31" xr3:uid="{ACB400C1-6E03-4981-87BA-B8F448E33609}" name="Eure-et-Loir" dataDxfId="106"/>
-    <tableColumn id="32" xr3:uid="{A0010EA8-88F5-4BFB-B5FD-DB4C1FABC9D3}" name="Finistère" dataDxfId="105"/>
-    <tableColumn id="33" xr3:uid="{2ADE7994-0D31-415C-8D5B-D744ED5FC46D}" name="Gard" dataDxfId="104"/>
-    <tableColumn id="34" xr3:uid="{F32DFC87-B65E-49EF-B7E1-11E14D457DE6}" name="Gers" dataDxfId="103"/>
-    <tableColumn id="35" xr3:uid="{E89AFA6C-B45A-4F39-8C1F-887DC31F47EE}" name="Gironde" dataDxfId="102"/>
-    <tableColumn id="36" xr3:uid="{F70D1BA5-1060-4BA9-ABA1-31FAC34E0047}" name="Guadeloupe" dataDxfId="101"/>
-    <tableColumn id="37" xr3:uid="{D7ACBB48-BDC9-40B5-85DF-955943C06392}" name="Guyane" dataDxfId="100"/>
-    <tableColumn id="38" xr3:uid="{1E811BA7-7958-4A55-B924-92B9CAAD10C3}" name="Haut-Rhin" dataDxfId="99"/>
-    <tableColumn id="39" xr3:uid="{42C1C79F-8BD5-451D-964B-E28BCEFE7953}" name="Haute-Corse" dataDxfId="98"/>
-    <tableColumn id="40" xr3:uid="{36B4C0CB-2FA0-49EF-A59E-044A2619FEA4}" name="Haute-Garonne" dataDxfId="97"/>
-    <tableColumn id="41" xr3:uid="{68868B2E-E899-4D1C-8A67-2BF42A4C0C7D}" name="Haute-Loire" dataDxfId="96"/>
-    <tableColumn id="42" xr3:uid="{8CF70388-25A1-4E51-9FA3-3FC90E6309F3}" name="Haute-Marne" dataDxfId="95"/>
-    <tableColumn id="43" xr3:uid="{9991CD78-264A-4A0E-B252-821C90984B96}" name="Haute-Savoie" dataDxfId="94"/>
-    <tableColumn id="44" xr3:uid="{3637CF11-C187-4C1B-86AC-4F1ACA2231EA}" name="Haute-Saône" dataDxfId="93"/>
-    <tableColumn id="45" xr3:uid="{DA60368F-7801-4AD2-A019-3A82A688E535}" name="Haute-Vienne" dataDxfId="92"/>
-    <tableColumn id="46" xr3:uid="{C71AF716-FD77-4BF7-9368-235F16A1C1BD}" name="Hautes-Alpes" dataDxfId="91"/>
-    <tableColumn id="47" xr3:uid="{A243BC10-75CC-417D-9769-08929D257A8E}" name="Hautes-Pyrénées" dataDxfId="90"/>
-    <tableColumn id="48" xr3:uid="{95485102-7BF1-4CA6-B9D3-A945950FE1C5}" name="Hauts-de-Seine" dataDxfId="89"/>
-    <tableColumn id="49" xr3:uid="{626F728A-8CED-4237-ACD8-173371128A6D}" name="Hérault" dataDxfId="88"/>
-    <tableColumn id="50" xr3:uid="{B3372E9D-DC31-44AC-AD67-391C434BA5A7}" name="Ille-et-Vilaine" dataDxfId="87"/>
-    <tableColumn id="51" xr3:uid="{C57C9F4E-E269-436B-9148-64D2617A6A0F}" name="Indre" dataDxfId="86"/>
-    <tableColumn id="52" xr3:uid="{930C842F-613C-4EF1-856D-4F8A4EEA27B1}" name="Indre-et-Loire" dataDxfId="85"/>
-    <tableColumn id="53" xr3:uid="{F0F1FA28-C979-4CFB-A9C6-F1D651653689}" name="Isère" dataDxfId="84"/>
-    <tableColumn id="54" xr3:uid="{DA1C3045-CA08-4978-94C7-1384C923C1AF}" name="Jura" dataDxfId="83"/>
-    <tableColumn id="55" xr3:uid="{66C3EF42-EC88-44E2-B499-91050A5AE7C2}" name="La Réunion" dataDxfId="82"/>
-    <tableColumn id="56" xr3:uid="{66BD0218-2122-4260-92EE-41C899CDA3D3}" name="Landes" dataDxfId="81"/>
-    <tableColumn id="57" xr3:uid="{C6E2131D-E8CB-4692-999D-B039F41FEB19}" name="Loir-et-Cher" dataDxfId="80"/>
-    <tableColumn id="58" xr3:uid="{B66AF8C5-F3D3-48F2-B43A-463E2F7637C0}" name="Loire" dataDxfId="79"/>
-    <tableColumn id="59" xr3:uid="{362337F0-580F-495C-A781-45B4AC518F27}" name="Loire-Atlantique" dataDxfId="78"/>
-    <tableColumn id="60" xr3:uid="{E5983660-13C2-4043-9C61-6114CFDA4FB3}" name="Loiret" dataDxfId="77"/>
-    <tableColumn id="61" xr3:uid="{7367AEC2-3CF6-440F-A751-C827CE21281A}" name="Lot" dataDxfId="76"/>
-    <tableColumn id="62" xr3:uid="{8DA875A8-2AC5-448C-927A-EF1AF6AA701D}" name="Lot-et-Garonne" dataDxfId="75"/>
-    <tableColumn id="63" xr3:uid="{B12F99B3-5CE8-4437-93A2-337B5CE3E3D6}" name="Lozère" dataDxfId="74"/>
-    <tableColumn id="64" xr3:uid="{C2D741F6-1BFC-4A87-AFAD-15BF34472A60}" name="Maine-et-Loire" dataDxfId="73"/>
-    <tableColumn id="65" xr3:uid="{0B5DC99E-83E2-40E2-9D1B-542EA8AF1BFB}" name="Manche" dataDxfId="72"/>
-    <tableColumn id="66" xr3:uid="{6D9BA7E3-D4FA-4D80-AC2C-C1EE0A28E8BC}" name="Marne" dataDxfId="71"/>
-    <tableColumn id="67" xr3:uid="{BE64437B-D56F-4EDF-9566-2062756F28EC}" name="Martinique" dataDxfId="70"/>
-    <tableColumn id="68" xr3:uid="{9E0E8A9B-5542-4E01-81BC-F4893C0F577C}" name="Mayenne" dataDxfId="69"/>
-    <tableColumn id="69" xr3:uid="{4780D916-1371-49C9-9A6B-4CE2B1B53788}" name="Mayotte" dataDxfId="68"/>
-    <tableColumn id="70" xr3:uid="{AD27B474-7A9C-42FB-9772-B251CB0917EB}" name="Meurthe-et-Moselle" dataDxfId="67"/>
-    <tableColumn id="71" xr3:uid="{9F7BF458-8D2B-4FD9-926D-C13FB3A04719}" name="Meuse" dataDxfId="66"/>
-    <tableColumn id="72" xr3:uid="{52B891CC-8E03-41FE-9F77-CBE77B3A03CF}" name="Morbihan" dataDxfId="65"/>
-    <tableColumn id="73" xr3:uid="{FB978F30-7986-44F8-85FB-D588B406A6E1}" name="Moselle" dataDxfId="64"/>
-    <tableColumn id="74" xr3:uid="{92789DCD-1A55-4B00-987E-DBB23D1D0F63}" name="Nièvre" dataDxfId="63"/>
-    <tableColumn id="75" xr3:uid="{0FFAE2BE-49C3-407A-B7E7-9D52C63CC2C5}" name="Nord" dataDxfId="62"/>
-    <tableColumn id="76" xr3:uid="{14DD721D-038E-44F9-8312-7D1F237E494C}" name="Nouvelle-Calédonie" dataDxfId="61"/>
-    <tableColumn id="77" xr3:uid="{2EABB539-5263-48C8-8503-B19DA097C2E4}" name="Oise" dataDxfId="60"/>
-    <tableColumn id="78" xr3:uid="{61BB17DF-8BE3-4A1F-9BF9-0F78A579D402}" name="Orne" dataDxfId="59"/>
-    <tableColumn id="79" xr3:uid="{7E1A73C9-5329-4A1B-BB24-E564C871B552}" name="Paris" dataDxfId="58"/>
-    <tableColumn id="80" xr3:uid="{167D2C08-5614-42CD-8602-43F57CBA5066}" name="Pas-de-Calais" dataDxfId="57"/>
-    <tableColumn id="81" xr3:uid="{4E43FC3C-CDE7-47A4-A9D3-AE331493D5BC}" name="Polynésie française" dataDxfId="56"/>
-    <tableColumn id="82" xr3:uid="{B48AACFC-9FB2-4061-9961-7DDFF5B9C01A}" name="Puy-de-Dôme" dataDxfId="55"/>
-    <tableColumn id="83" xr3:uid="{A4A947CB-A290-4751-9C66-2AE78C2592C4}" name="Pyrénées-Atlantiques" dataDxfId="54"/>
-    <tableColumn id="84" xr3:uid="{6C049822-5AEF-43DF-B8DB-B54B8E0E1BE9}" name="Pyrénées-Orientales" dataDxfId="53"/>
-    <tableColumn id="85" xr3:uid="{AD51126C-4807-4EE8-9CC6-78FCF3F7C2B7}" name="Rhône" dataDxfId="52"/>
-    <tableColumn id="86" xr3:uid="{AB7D602C-E6BF-4010-BEEB-DE99BBF54B21}" name="Saint-Martin/Saint-Barthélemy" dataDxfId="51"/>
-    <tableColumn id="87" xr3:uid="{829002FC-98F1-4C0D-9EFF-6DC27A17654B}" name="Saint-Pierre-et-Miquelon" dataDxfId="50"/>
-    <tableColumn id="88" xr3:uid="{2D3BA051-2706-4F01-B69D-33879F7775CE}" name="Sarthe" dataDxfId="49"/>
-    <tableColumn id="89" xr3:uid="{0BF0643A-FD9D-4B39-BB9F-A9485274258B}" name="Savoie" dataDxfId="48"/>
-    <tableColumn id="90" xr3:uid="{DC19E2F3-A469-445C-937E-246806A4E0E4}" name="Saône-et-Loire" dataDxfId="47"/>
-    <tableColumn id="91" xr3:uid="{48D358ED-27D4-49DD-B90A-9706EE396878}" name="Seine-Maritime" dataDxfId="46"/>
-    <tableColumn id="92" xr3:uid="{E3BF594D-AA75-4FAF-8978-4E29A613CD1B}" name="Seine-Saint-Denis" dataDxfId="45"/>
-    <tableColumn id="93" xr3:uid="{E613C3F7-F72A-49AA-9599-74960AE9D189}" name="Seine-et-Marne" dataDxfId="44"/>
-    <tableColumn id="94" xr3:uid="{A7E14350-E02D-4913-B421-01C042FD6F3C}" name="Somme" dataDxfId="43"/>
-    <tableColumn id="95" xr3:uid="{B0E3246A-EF68-4157-BBAC-47AFED718F92}" name="Tarn" dataDxfId="42"/>
-    <tableColumn id="96" xr3:uid="{C8C7BB4A-10F5-4B5E-B66A-CC1F50DE1705}" name="Tarn-et-Garonne" dataDxfId="41"/>
-    <tableColumn id="97" xr3:uid="{8A7EE812-37A9-4191-8FFB-FE55A42A3C1D}" name="Territoire de Belfort" dataDxfId="40"/>
-    <tableColumn id="98" xr3:uid="{EEA62222-52ED-41E3-94EA-596CAFE64406}" name="Val-d'Oise" dataDxfId="39"/>
-    <tableColumn id="99" xr3:uid="{C3DC370D-EEF7-4AEA-B34C-B8F131564070}" name="Val-de-Marne" dataDxfId="38"/>
-    <tableColumn id="100" xr3:uid="{DAE410B7-34F4-407F-A6E1-A7077D31F603}" name="Var" dataDxfId="37"/>
-    <tableColumn id="101" xr3:uid="{814759AF-9F4E-45AF-AD4F-5BD76A013DFB}" name="Vaucluse" dataDxfId="36"/>
-    <tableColumn id="102" xr3:uid="{029998F9-4C24-4C24-B3E6-99C9DA70C54C}" name="Vendée" dataDxfId="35"/>
-    <tableColumn id="103" xr3:uid="{D9196820-BAC6-4776-9454-9135203F4B51}" name="Vienne" dataDxfId="34"/>
-    <tableColumn id="104" xr3:uid="{88A467E4-5EE2-47C5-85F8-B3B5FB1ED660}" name="Vosges" dataDxfId="33"/>
-    <tableColumn id="105" xr3:uid="{390ABB01-0672-4710-B5F2-D3CD090AC4AA}" name="Wallis et Futuna" dataDxfId="32"/>
-    <tableColumn id="106" xr3:uid="{709EE3EF-82C4-41BD-8015-EF7F11859715}" name="Yonne" dataDxfId="31"/>
-    <tableColumn id="107" xr3:uid="{35295217-2F2D-401F-8207-0270293A6FA3}" name="Yvelines" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{27C8E1A7-4DD3-497E-9BB7-9E0EE471B6E9}" name="Candidate" dataDxfId="112"/>
+    <tableColumn id="2" xr3:uid="{8CCB92DA-03BE-4E04-9048-217E624457FE}" name="Ain" dataDxfId="111"/>
+    <tableColumn id="3" xr3:uid="{5850EA8D-19C4-464A-803C-AE76ED004BD3}" name="Aisne" dataDxfId="110"/>
+    <tableColumn id="4" xr3:uid="{A6D7EBC4-3FE3-4221-8CCA-78E0740E2B64}" name="Allier" dataDxfId="109"/>
+    <tableColumn id="5" xr3:uid="{BE876166-4E7F-40FA-968C-02CBE720939A}" name="Alpes-Maritimes" dataDxfId="108"/>
+    <tableColumn id="6" xr3:uid="{232532A6-0C44-4E86-A5AF-A317ECD29C04}" name="Alpes-de-Haute-Provence" dataDxfId="107"/>
+    <tableColumn id="7" xr3:uid="{2373349C-D894-424D-AA87-AEE39F79AD05}" name="Ardennes" dataDxfId="106"/>
+    <tableColumn id="8" xr3:uid="{2B73B324-EE11-4018-9BF9-84682AC1F105}" name="Ardèche" dataDxfId="105"/>
+    <tableColumn id="9" xr3:uid="{16372E34-A8F2-4A61-8F28-063FA267BC65}" name="Ariège" dataDxfId="104"/>
+    <tableColumn id="10" xr3:uid="{682605AC-2360-4778-9C99-8D2E17716ED5}" name="Aube" dataDxfId="103"/>
+    <tableColumn id="11" xr3:uid="{981C5C21-7AC7-47EA-A861-ADA53019D2EE}" name="Aude" dataDxfId="102"/>
+    <tableColumn id="12" xr3:uid="{8048A4F9-B569-4139-A8EF-B7CD7DC9AB56}" name="Aveyron" dataDxfId="101"/>
+    <tableColumn id="13" xr3:uid="{CAF3796D-7307-4506-8316-970783B565DE}" name="Bas-Rhin" dataDxfId="100"/>
+    <tableColumn id="14" xr3:uid="{92A27818-DB05-44C6-BDD3-489379907650}" name="Bouches-du-Rhône" dataDxfId="99"/>
+    <tableColumn id="15" xr3:uid="{09D411A4-73D7-4592-8926-BEBAF46A4E4F}" name="Calvados" dataDxfId="98"/>
+    <tableColumn id="16" xr3:uid="{3F66DE9E-989E-4D21-B8FE-5AB647243D04}" name="Cantal" dataDxfId="97"/>
+    <tableColumn id="17" xr3:uid="{A7691DC8-030B-4E6F-B599-4D694CC66BC2}" name="Charente" dataDxfId="96"/>
+    <tableColumn id="18" xr3:uid="{4312157F-5109-415F-BF4F-A5D40DCEF34A}" name="Charente-Maritime" dataDxfId="95"/>
+    <tableColumn id="19" xr3:uid="{1335A6BC-A79F-4F25-937E-7411352074B7}" name="Cher" dataDxfId="94"/>
+    <tableColumn id="20" xr3:uid="{ABB30B80-C652-4182-A93D-AE336859C19F}" name="Corrèze" dataDxfId="93"/>
+    <tableColumn id="21" xr3:uid="{150B3246-C696-4D43-BC4C-053D447C0C48}" name="Corse-du-Sud" dataDxfId="92"/>
+    <tableColumn id="22" xr3:uid="{61704F7C-FB36-4160-90D1-9181EB7D489E}" name="Creuse" dataDxfId="91"/>
+    <tableColumn id="23" xr3:uid="{BBC4F1BA-8753-4F7E-9BFA-E8F4E262C658}" name="Côte-d'Or" dataDxfId="90"/>
+    <tableColumn id="24" xr3:uid="{25DB42A6-CECF-429D-B06D-C4428313548B}" name="Côtes-d'Armor" dataDxfId="89"/>
+    <tableColumn id="25" xr3:uid="{78B8BED2-E7C2-402C-A723-5EEE3BB04CDC}" name="Deux-Sèvres" dataDxfId="88"/>
+    <tableColumn id="26" xr3:uid="{56BEE575-2617-400C-A0AE-FB05670ACE71}" name="Dordogne" dataDxfId="87"/>
+    <tableColumn id="27" xr3:uid="{5425430B-1026-4534-A351-16430171312D}" name="Doubs" dataDxfId="86"/>
+    <tableColumn id="28" xr3:uid="{FDD5121D-C879-457B-A2DF-C83B7CC13CD0}" name="Drôme" dataDxfId="85"/>
+    <tableColumn id="29" xr3:uid="{7B72C5EC-FFEA-4EE7-9221-9450CC387071}" name="Essonne" dataDxfId="84"/>
+    <tableColumn id="30" xr3:uid="{9F6C6700-5FAB-454E-B2D8-4065D439F10E}" name="Eure" dataDxfId="83"/>
+    <tableColumn id="31" xr3:uid="{ACB400C1-6E03-4981-87BA-B8F448E33609}" name="Eure-et-Loir" dataDxfId="82"/>
+    <tableColumn id="32" xr3:uid="{A0010EA8-88F5-4BFB-B5FD-DB4C1FABC9D3}" name="Finistère" dataDxfId="81"/>
+    <tableColumn id="33" xr3:uid="{2ADE7994-0D31-415C-8D5B-D744ED5FC46D}" name="Gard" dataDxfId="80"/>
+    <tableColumn id="34" xr3:uid="{F32DFC87-B65E-49EF-B7E1-11E14D457DE6}" name="Gers" dataDxfId="79"/>
+    <tableColumn id="35" xr3:uid="{E89AFA6C-B45A-4F39-8C1F-887DC31F47EE}" name="Gironde" dataDxfId="78"/>
+    <tableColumn id="36" xr3:uid="{F70D1BA5-1060-4BA9-ABA1-31FAC34E0047}" name="Guadeloupe" dataDxfId="77"/>
+    <tableColumn id="37" xr3:uid="{D7ACBB48-BDC9-40B5-85DF-955943C06392}" name="Guyane" dataDxfId="76"/>
+    <tableColumn id="38" xr3:uid="{1E811BA7-7958-4A55-B924-92B9CAAD10C3}" name="Haut-Rhin" dataDxfId="75"/>
+    <tableColumn id="39" xr3:uid="{42C1C79F-8BD5-451D-964B-E28BCEFE7953}" name="Haute-Corse" dataDxfId="74"/>
+    <tableColumn id="40" xr3:uid="{36B4C0CB-2FA0-49EF-A59E-044A2619FEA4}" name="Haute-Garonne" dataDxfId="73"/>
+    <tableColumn id="41" xr3:uid="{68868B2E-E899-4D1C-8A67-2BF42A4C0C7D}" name="Haute-Loire" dataDxfId="72"/>
+    <tableColumn id="42" xr3:uid="{8CF70388-25A1-4E51-9FA3-3FC90E6309F3}" name="Haute-Marne" dataDxfId="71"/>
+    <tableColumn id="43" xr3:uid="{9991CD78-264A-4A0E-B252-821C90984B96}" name="Haute-Savoie" dataDxfId="70"/>
+    <tableColumn id="44" xr3:uid="{3637CF11-C187-4C1B-86AC-4F1ACA2231EA}" name="Haute-Saône" dataDxfId="69"/>
+    <tableColumn id="45" xr3:uid="{DA60368F-7801-4AD2-A019-3A82A688E535}" name="Haute-Vienne" dataDxfId="68"/>
+    <tableColumn id="46" xr3:uid="{C71AF716-FD77-4BF7-9368-235F16A1C1BD}" name="Hautes-Alpes" dataDxfId="67"/>
+    <tableColumn id="47" xr3:uid="{A243BC10-75CC-417D-9769-08929D257A8E}" name="Hautes-Pyrénées" dataDxfId="66"/>
+    <tableColumn id="48" xr3:uid="{95485102-7BF1-4CA6-B9D3-A945950FE1C5}" name="Hauts-de-Seine" dataDxfId="65"/>
+    <tableColumn id="49" xr3:uid="{626F728A-8CED-4237-ACD8-173371128A6D}" name="Hérault" dataDxfId="64"/>
+    <tableColumn id="50" xr3:uid="{B3372E9D-DC31-44AC-AD67-391C434BA5A7}" name="Ille-et-Vilaine" dataDxfId="63"/>
+    <tableColumn id="51" xr3:uid="{C57C9F4E-E269-436B-9148-64D2617A6A0F}" name="Indre" dataDxfId="62"/>
+    <tableColumn id="52" xr3:uid="{930C842F-613C-4EF1-856D-4F8A4EEA27B1}" name="Indre-et-Loire" dataDxfId="61"/>
+    <tableColumn id="53" xr3:uid="{F0F1FA28-C979-4CFB-A9C6-F1D651653689}" name="Isère" dataDxfId="60"/>
+    <tableColumn id="54" xr3:uid="{DA1C3045-CA08-4978-94C7-1384C923C1AF}" name="Jura" dataDxfId="59"/>
+    <tableColumn id="55" xr3:uid="{66C3EF42-EC88-44E2-B499-91050A5AE7C2}" name="La Réunion" dataDxfId="58"/>
+    <tableColumn id="56" xr3:uid="{66BD0218-2122-4260-92EE-41C899CDA3D3}" name="Landes" dataDxfId="57"/>
+    <tableColumn id="57" xr3:uid="{C6E2131D-E8CB-4692-999D-B039F41FEB19}" name="Loir-et-Cher" dataDxfId="56"/>
+    <tableColumn id="58" xr3:uid="{B66AF8C5-F3D3-48F2-B43A-463E2F7637C0}" name="Loire" dataDxfId="55"/>
+    <tableColumn id="59" xr3:uid="{362337F0-580F-495C-A781-45B4AC518F27}" name="Loire-Atlantique" dataDxfId="54"/>
+    <tableColumn id="60" xr3:uid="{E5983660-13C2-4043-9C61-6114CFDA4FB3}" name="Loiret" dataDxfId="53"/>
+    <tableColumn id="61" xr3:uid="{7367AEC2-3CF6-440F-A751-C827CE21281A}" name="Lot" dataDxfId="52"/>
+    <tableColumn id="62" xr3:uid="{8DA875A8-2AC5-448C-927A-EF1AF6AA701D}" name="Lot-et-Garonne" dataDxfId="51"/>
+    <tableColumn id="63" xr3:uid="{B12F99B3-5CE8-4437-93A2-337B5CE3E3D6}" name="Lozère" dataDxfId="50"/>
+    <tableColumn id="64" xr3:uid="{C2D741F6-1BFC-4A87-AFAD-15BF34472A60}" name="Maine-et-Loire" dataDxfId="49"/>
+    <tableColumn id="65" xr3:uid="{0B5DC99E-83E2-40E2-9D1B-542EA8AF1BFB}" name="Manche" dataDxfId="48"/>
+    <tableColumn id="66" xr3:uid="{6D9BA7E3-D4FA-4D80-AC2C-C1EE0A28E8BC}" name="Marne" dataDxfId="47"/>
+    <tableColumn id="67" xr3:uid="{BE64437B-D56F-4EDF-9566-2062756F28EC}" name="Martinique" dataDxfId="46"/>
+    <tableColumn id="68" xr3:uid="{9E0E8A9B-5542-4E01-81BC-F4893C0F577C}" name="Mayenne" dataDxfId="45"/>
+    <tableColumn id="69" xr3:uid="{4780D916-1371-49C9-9A6B-4CE2B1B53788}" name="Mayotte" dataDxfId="44"/>
+    <tableColumn id="70" xr3:uid="{AD27B474-7A9C-42FB-9772-B251CB0917EB}" name="Meurthe-et-Moselle" dataDxfId="43"/>
+    <tableColumn id="71" xr3:uid="{9F7BF458-8D2B-4FD9-926D-C13FB3A04719}" name="Meuse" dataDxfId="42"/>
+    <tableColumn id="72" xr3:uid="{52B891CC-8E03-41FE-9F77-CBE77B3A03CF}" name="Morbihan" dataDxfId="41"/>
+    <tableColumn id="73" xr3:uid="{FB978F30-7986-44F8-85FB-D588B406A6E1}" name="Moselle" dataDxfId="40"/>
+    <tableColumn id="74" xr3:uid="{92789DCD-1A55-4B00-987E-DBB23D1D0F63}" name="Nièvre" dataDxfId="39"/>
+    <tableColumn id="75" xr3:uid="{0FFAE2BE-49C3-407A-B7E7-9D52C63CC2C5}" name="Nord" dataDxfId="38"/>
+    <tableColumn id="76" xr3:uid="{14DD721D-038E-44F9-8312-7D1F237E494C}" name="Nouvelle-Calédonie" dataDxfId="37"/>
+    <tableColumn id="77" xr3:uid="{2EABB539-5263-48C8-8503-B19DA097C2E4}" name="Oise" dataDxfId="36"/>
+    <tableColumn id="78" xr3:uid="{61BB17DF-8BE3-4A1F-9BF9-0F78A579D402}" name="Orne" dataDxfId="35"/>
+    <tableColumn id="79" xr3:uid="{7E1A73C9-5329-4A1B-BB24-E564C871B552}" name="Paris" dataDxfId="34"/>
+    <tableColumn id="80" xr3:uid="{167D2C08-5614-42CD-8602-43F57CBA5066}" name="Pas-de-Calais" dataDxfId="33"/>
+    <tableColumn id="81" xr3:uid="{4E43FC3C-CDE7-47A4-A9D3-AE331493D5BC}" name="Polynésie française" dataDxfId="32"/>
+    <tableColumn id="82" xr3:uid="{B48AACFC-9FB2-4061-9961-7DDFF5B9C01A}" name="Puy-de-Dôme" dataDxfId="31"/>
+    <tableColumn id="83" xr3:uid="{A4A947CB-A290-4751-9C66-2AE78C2592C4}" name="Pyrénées-Atlantiques" dataDxfId="30"/>
+    <tableColumn id="84" xr3:uid="{6C049822-5AEF-43DF-B8DB-B54B8E0E1BE9}" name="Pyrénées-Orientales" dataDxfId="29"/>
+    <tableColumn id="85" xr3:uid="{AD51126C-4807-4EE8-9CC6-78FCF3F7C2B7}" name="Rhône" dataDxfId="28"/>
+    <tableColumn id="86" xr3:uid="{AB7D602C-E6BF-4010-BEEB-DE99BBF54B21}" name="Saint-Martin/Saint-Barthélemy" dataDxfId="27"/>
+    <tableColumn id="87" xr3:uid="{829002FC-98F1-4C0D-9EFF-6DC27A17654B}" name="Saint-Pierre-et-Miquelon" dataDxfId="26"/>
+    <tableColumn id="88" xr3:uid="{2D3BA051-2706-4F01-B69D-33879F7775CE}" name="Sarthe" dataDxfId="25"/>
+    <tableColumn id="89" xr3:uid="{0BF0643A-FD9D-4B39-BB9F-A9485274258B}" name="Savoie" dataDxfId="24"/>
+    <tableColumn id="90" xr3:uid="{DC19E2F3-A469-445C-937E-246806A4E0E4}" name="Saône-et-Loire" dataDxfId="23"/>
+    <tableColumn id="91" xr3:uid="{48D358ED-27D4-49DD-B90A-9706EE396878}" name="Seine-Maritime" dataDxfId="22"/>
+    <tableColumn id="92" xr3:uid="{E3BF594D-AA75-4FAF-8978-4E29A613CD1B}" name="Seine-Saint-Denis" dataDxfId="21"/>
+    <tableColumn id="93" xr3:uid="{E613C3F7-F72A-49AA-9599-74960AE9D189}" name="Seine-et-Marne" dataDxfId="20"/>
+    <tableColumn id="94" xr3:uid="{A7E14350-E02D-4913-B421-01C042FD6F3C}" name="Somme" dataDxfId="19"/>
+    <tableColumn id="95" xr3:uid="{B0E3246A-EF68-4157-BBAC-47AFED718F92}" name="Tarn" dataDxfId="18"/>
+    <tableColumn id="96" xr3:uid="{C8C7BB4A-10F5-4B5E-B66A-CC1F50DE1705}" name="Tarn-et-Garonne" dataDxfId="17"/>
+    <tableColumn id="97" xr3:uid="{8A7EE812-37A9-4191-8FFB-FE55A42A3C1D}" name="Territoire de Belfort" dataDxfId="16"/>
+    <tableColumn id="98" xr3:uid="{EEA62222-52ED-41E3-94EA-596CAFE64406}" name="Val-d'Oise" dataDxfId="15"/>
+    <tableColumn id="99" xr3:uid="{C3DC370D-EEF7-4AEA-B34C-B8F131564070}" name="Val-de-Marne" dataDxfId="14"/>
+    <tableColumn id="100" xr3:uid="{DAE410B7-34F4-407F-A6E1-A7077D31F603}" name="Var" dataDxfId="13"/>
+    <tableColumn id="101" xr3:uid="{814759AF-9F4E-45AF-AD4F-5BD76A013DFB}" name="Vaucluse" dataDxfId="12"/>
+    <tableColumn id="102" xr3:uid="{029998F9-4C24-4C24-B3E6-99C9DA70C54C}" name="Vendée" dataDxfId="11"/>
+    <tableColumn id="103" xr3:uid="{D9196820-BAC6-4776-9454-9135203F4B51}" name="Vienne" dataDxfId="10"/>
+    <tableColumn id="104" xr3:uid="{88A467E4-5EE2-47C5-85F8-B3B5FB1ED660}" name="Vosges" dataDxfId="9"/>
+    <tableColumn id="105" xr3:uid="{390ABB01-0672-4710-B5F2-D3CD090AC4AA}" name="Wallis et Futuna" dataDxfId="8"/>
+    <tableColumn id="106" xr3:uid="{709EE3EF-82C4-41BD-8015-EF7F11859715}" name="Yonne" dataDxfId="7"/>
+    <tableColumn id="107" xr3:uid="{35295217-2F2D-401F-8207-0270293A6FA3}" name="Yvelines" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6964,14 +6881,242 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE4100C5-6FB3-4A66-9859-158C80A03F7E}">
+  <dimension ref="F4:S17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="H4" s="48" t="s">
+        <v>135</v>
+      </c>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="48"/>
+    </row>
+    <row r="5" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
+      <c r="O5" s="48"/>
+      <c r="P5" s="48"/>
+      <c r="Q5" s="48"/>
+    </row>
+    <row r="6" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="48"/>
+      <c r="P6" s="48"/>
+      <c r="Q6" s="48"/>
+    </row>
+    <row r="7" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="48"/>
+      <c r="N7" s="48"/>
+      <c r="O7" s="48"/>
+      <c r="P7" s="48"/>
+      <c r="Q7" s="48"/>
+    </row>
+    <row r="8" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="48"/>
+      <c r="N8" s="48"/>
+      <c r="O8" s="48"/>
+      <c r="P8" s="48"/>
+      <c r="Q8" s="48"/>
+    </row>
+    <row r="9" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="48"/>
+      <c r="L9" s="48"/>
+      <c r="M9" s="48"/>
+      <c r="N9" s="48"/>
+      <c r="O9" s="48"/>
+      <c r="P9" s="48"/>
+      <c r="Q9" s="48"/>
+    </row>
+    <row r="10" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="47"/>
+      <c r="M10" s="47"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="47"/>
+      <c r="P10" s="47"/>
+      <c r="Q10" s="47"/>
+      <c r="R10" s="47"/>
+      <c r="S10" s="47"/>
+    </row>
+    <row r="11" spans="6:19" ht="18" x14ac:dyDescent="0.35">
+      <c r="F11" s="49" t="s">
+        <v>136</v>
+      </c>
+      <c r="G11" s="49"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="49"/>
+      <c r="N11" s="49"/>
+      <c r="O11" s="47"/>
+      <c r="P11" s="47"/>
+      <c r="Q11" s="47"/>
+      <c r="R11" s="47"/>
+      <c r="S11" s="47"/>
+    </row>
+    <row r="12" spans="6:19" x14ac:dyDescent="0.3">
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="47"/>
+      <c r="P12" s="47"/>
+      <c r="Q12" s="47"/>
+      <c r="R12" s="47"/>
+      <c r="S12" s="47"/>
+    </row>
+    <row r="13" spans="6:19" ht="21" x14ac:dyDescent="0.4">
+      <c r="F13" s="54"/>
+      <c r="G13" s="50" t="str">
+        <f>HYPERLINK("#'Data Searching Tool'!D10","1) Data Searching Tool")</f>
+        <v>1) Data Searching Tool</v>
+      </c>
+      <c r="H13" s="51"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="51"/>
+      <c r="K13" s="51"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="47"/>
+      <c r="N13" s="47"/>
+      <c r="O13" s="47"/>
+      <c r="P13" s="47"/>
+      <c r="Q13" s="47"/>
+      <c r="R13" s="47"/>
+      <c r="S13" s="47"/>
+    </row>
+    <row r="14" spans="6:19" ht="21" x14ac:dyDescent="0.4">
+      <c r="F14" s="54"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="53"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="47"/>
+      <c r="N14" s="47"/>
+      <c r="O14" s="47"/>
+      <c r="P14" s="47"/>
+      <c r="Q14" s="47"/>
+      <c r="R14" s="47"/>
+      <c r="S14" s="47"/>
+    </row>
+    <row r="15" spans="6:19" ht="21" x14ac:dyDescent="0.4">
+      <c r="F15" s="54"/>
+      <c r="G15" s="50" t="str">
+        <f>HYPERLINK("#'Data'!A1","2) Raw Data Table")</f>
+        <v>2) Raw Data Table</v>
+      </c>
+      <c r="H15" s="51"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="51"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="47"/>
+      <c r="O15" s="47"/>
+      <c r="P15" s="47"/>
+      <c r="Q15" s="47"/>
+      <c r="R15" s="47"/>
+      <c r="S15" s="47"/>
+    </row>
+    <row r="16" spans="6:19" ht="21" x14ac:dyDescent="0.4">
+      <c r="F16" s="54"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="53"/>
+      <c r="K16" s="53"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="47"/>
+      <c r="O16" s="47"/>
+      <c r="P16" s="47"/>
+      <c r="Q16" s="47"/>
+      <c r="R16" s="47"/>
+      <c r="S16" s="47"/>
+    </row>
+    <row r="17" spans="6:11" ht="21" x14ac:dyDescent="0.4">
+      <c r="F17" s="55"/>
+      <c r="G17" s="50" t="str">
+        <f>HYPERLINK("#'Data Comparator Tool'!C4","3) Data Comparator Tool")</f>
+        <v>3) Data Comparator Tool</v>
+      </c>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="51"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="G17:K17"/>
+    <mergeCell ref="F11:N11"/>
+    <mergeCell ref="H4:Q9"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="G15:K15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53C41958-D55A-42F7-81EE-CEF64CB34796}">
-  <sheetPr>
-    <tabColor theme="6"/>
-  </sheetPr>
   <dimension ref="A3:DG182"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:F6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7024,99 +7169,104 @@
     <col min="110" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="46" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" s="46"/>
       <c r="H3" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="I3" s="36" t="s">
+      <c r="I3" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="38"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="35"/>
     </row>
-    <row r="4" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C4" s="36" t="s">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C4" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="40"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="37"/>
       <c r="H4" s="18"/>
-      <c r="I4" s="29" t="s">
+      <c r="I4" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="32"/>
+      <c r="Q4"/>
     </row>
-    <row r="5" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C5" s="22" t="str">
         <f>"Candidate: "&amp;IF(D5="", "(None selected)","")</f>
         <v xml:space="preserve">Candidate: </v>
       </c>
-      <c r="D5" s="41" t="s">
-        <v>107</v>
-      </c>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
+      <c r="D5" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
       <c r="H5" s="19"/>
-      <c r="I5" s="29" t="s">
+      <c r="I5" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="32"/>
     </row>
-    <row r="6" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C6" s="24" t="str">
         <f>"Department: "&amp;IF(D6="", "(None selected)","")</f>
         <v xml:space="preserve">Department: </v>
       </c>
-      <c r="D6" s="41" t="s">
-        <v>105</v>
-      </c>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
+      <c r="D6" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
       <c r="H6" s="23"/>
-      <c r="I6" s="29" t="s">
+      <c r="I6" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="32"/>
     </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="H7" s="21"/>
-      <c r="I7" s="29" t="s">
+      <c r="I7" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="32"/>
     </row>
-    <row r="8" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="H8" s="28"/>
-      <c r="I8" s="29" t="s">
+      <c r="I8" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="32"/>
     </row>
-    <row r="9" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="H9" s="27"/>
       <c r="I9" s="26"/>
       <c r="J9" s="26"/>
@@ -7125,7 +7275,7 @@
       <c r="M9" s="26"/>
       <c r="N9" s="26"/>
     </row>
-    <row r="10" spans="3:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="25" t="s">
         <v>128</v>
       </c>
@@ -7133,13 +7283,13 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="11" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C11" s="10" t="s">
         <v>119</v>
       </c>
       <c r="D11" s="16">
         <f ca="1">IF(D10="","No condition selected",IF(D5="",COUNTIFS(Table24[[Ain]:[Yvelines]],"&gt;="&amp;D10),COUNTIF(_xlfn.ANCHORARRAY(E42),"&gt;"&amp;D10)))</f>
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:110" customFormat="1" x14ac:dyDescent="0.3">
@@ -11056,24 +11206,20 @@
       </c>
     </row>
     <row r="37" spans="1:110" x14ac:dyDescent="0.3">
-      <c r="B37" s="32" t="s">
-        <v>130</v>
-      </c>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="32"/>
+      <c r="B37" s="44"/>
+      <c r="C37" s="44"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="44"/>
+      <c r="G37" s="44"/>
     </row>
     <row r="38" spans="1:110" x14ac:dyDescent="0.3">
-      <c r="B38" s="33" t="s">
-        <v>131</v>
-      </c>
-      <c r="C38" s="34"/>
-      <c r="D38" s="34"/>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
-      <c r="G38" s="35"/>
+      <c r="B38" s="45"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="45"/>
+      <c r="F38" s="45"/>
+      <c r="G38" s="45"/>
       <c r="H38" s="15"/>
       <c r="I38" s="15"/>
       <c r="J38" s="15"/>
@@ -11503,429 +11649,429 @@
       <c r="DF41" s="15"/>
     </row>
     <row r="42" spans="1:110" x14ac:dyDescent="0.3">
-      <c r="E42" s="49" cm="1">
+      <c r="E42" s="29" cm="1">
         <f t="array" aca="1" ref="E42:DF42" ca="1">IFERROR(IF(OFFSET(Table24[[Ain]:[Yvelines]],MATCH($D$5,Table24[Candidate],0)-1,0,1,COLUMNS(Table24[[#Headers],[Ain]:[Yvelines]]))&gt;D10,OFFSET(Table24[[Ain]:[Yvelines]],MATCH($D$5,Table24[Candidate],0)-1,0,1,COLUMNS(Table24[[#Headers],[Ain]:[Yvelines]])),0),0)</f>
         <v>0</v>
       </c>
-      <c r="F42" s="49">
+      <c r="F42" s="29">
         <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="G42" s="49">
+        <v>104677</v>
+      </c>
+      <c r="G42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="H42" s="49">
+      <c r="H42" s="29">
         <f ca="1"/>
-        <v>139966</v>
-      </c>
-      <c r="I42" s="49">
+        <v>149218</v>
+      </c>
+      <c r="I42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="J42" s="49">
+      <c r="J42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="K42" s="49">
+      <c r="K42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="L42" s="49">
+      <c r="L42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="M42" s="49">
+      <c r="M42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="N42" s="49">
+      <c r="N42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="O42" s="49">
+      <c r="O42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="P42" s="49">
+      <c r="P42" s="29">
         <f ca="1"/>
-        <v>177018</v>
-      </c>
-      <c r="Q42" s="49">
+        <v>145869</v>
+      </c>
+      <c r="Q42" s="29">
         <f ca="1"/>
-        <v>229038</v>
-      </c>
-      <c r="R42" s="49">
+        <v>264754</v>
+      </c>
+      <c r="R42" s="29">
         <f ca="1"/>
-        <v>120366</v>
-      </c>
-      <c r="S42" s="49">
+        <v>0</v>
+      </c>
+      <c r="S42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="T42" s="49">
+      <c r="T42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="U42" s="49">
+      <c r="U42" s="29">
         <f ca="1"/>
-        <v>113753</v>
-      </c>
-      <c r="V42" s="49">
+        <v>0</v>
+      </c>
+      <c r="V42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="W42" s="49">
+      <c r="W42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="X42" s="49">
+      <c r="X42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="Y42" s="49">
+      <c r="Y42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="Z42" s="49">
+      <c r="Z42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="AA42" s="49">
+      <c r="AA42" s="29">
         <f ca="1"/>
-        <v>113654</v>
-      </c>
-      <c r="AB42" s="49">
+        <v>0</v>
+      </c>
+      <c r="AB42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="AC42" s="49">
+      <c r="AC42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="AD42" s="49">
+      <c r="AD42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="AE42" s="49">
+      <c r="AE42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="AF42" s="49">
+      <c r="AF42" s="29">
         <f ca="1"/>
-        <v>164503</v>
-      </c>
-      <c r="AG42" s="49">
+        <v>105862</v>
+      </c>
+      <c r="AG42" s="29">
         <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="AH42" s="49">
+        <v>102951</v>
+      </c>
+      <c r="AH42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="AI42" s="49">
+      <c r="AI42" s="29">
         <f ca="1"/>
-        <v>174892</v>
-      </c>
-      <c r="AJ42" s="49">
+        <v>100890</v>
+      </c>
+      <c r="AJ42" s="29">
         <f ca="1"/>
-        <v>0</v>
-      </c>
-      <c r="AK42" s="49">
+        <v>121478</v>
+      </c>
+      <c r="AK42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="AL42" s="49">
+      <c r="AL42" s="29">
         <f ca="1"/>
-        <v>256179</v>
-      </c>
-      <c r="AM42" s="49">
+        <v>191542</v>
+      </c>
+      <c r="AM42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="AN42" s="49">
+      <c r="AN42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="AO42" s="49">
+      <c r="AO42" s="29">
         <f ca="1"/>
-        <v>107244</v>
-      </c>
-      <c r="AP42" s="49">
+        <v>106930</v>
+      </c>
+      <c r="AP42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="AQ42" s="49">
+      <c r="AQ42" s="29">
         <f ca="1"/>
-        <v>197049</v>
-      </c>
-      <c r="AR42" s="49">
+        <v>133411</v>
+      </c>
+      <c r="AR42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="AS42" s="49">
+      <c r="AS42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="AT42" s="49">
+      <c r="AT42" s="29">
         <f ca="1"/>
-        <v>130422</v>
-      </c>
-      <c r="AU42" s="49">
+        <v>0</v>
+      </c>
+      <c r="AU42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="AV42" s="49">
+      <c r="AV42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="AW42" s="49">
+      <c r="AW42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="AX42" s="49">
+      <c r="AX42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="AY42" s="49">
+      <c r="AY42" s="29">
         <f ca="1"/>
-        <v>287494</v>
-      </c>
-      <c r="AZ42" s="49">
+        <v>0</v>
+      </c>
+      <c r="AZ42" s="29">
         <f ca="1"/>
-        <v>142302</v>
-      </c>
-      <c r="BA42" s="49">
+        <v>165729</v>
+      </c>
+      <c r="BA42" s="29">
         <f ca="1"/>
-        <v>205894</v>
-      </c>
-      <c r="BB42" s="49">
+        <v>101797</v>
+      </c>
+      <c r="BB42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="BC42" s="49">
+      <c r="BC42" s="29">
         <f ca="1"/>
-        <v>101503</v>
-      </c>
-      <c r="BD42" s="49">
+        <v>0</v>
+      </c>
+      <c r="BD42" s="29">
         <f ca="1"/>
-        <v>180553</v>
-      </c>
-      <c r="BE42" s="49">
+        <v>154889</v>
+      </c>
+      <c r="BE42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="BF42" s="49">
+      <c r="BF42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="BG42" s="49">
+      <c r="BG42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="BH42" s="49">
+      <c r="BH42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="BI42" s="49">
+      <c r="BI42" s="29">
         <f ca="1"/>
-        <v>104096</v>
-      </c>
-      <c r="BJ42" s="49">
+        <v>0</v>
+      </c>
+      <c r="BJ42" s="29">
         <f ca="1"/>
-        <v>256609</v>
-      </c>
-      <c r="BK42" s="49">
+        <v>135702</v>
+      </c>
+      <c r="BK42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="BL42" s="49">
+      <c r="BL42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="BM42" s="49">
+      <c r="BM42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="BN42" s="49">
+      <c r="BN42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="BO42" s="49">
+      <c r="BO42" s="29">
         <f ca="1"/>
-        <v>157086</v>
-      </c>
-      <c r="BP42" s="49">
+        <v>0</v>
+      </c>
+      <c r="BP42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="BQ42" s="49">
+      <c r="BQ42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="BR42" s="49">
+      <c r="BR42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="BS42" s="49">
+      <c r="BS42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="BT42" s="49">
+      <c r="BT42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="BU42" s="49">
+      <c r="BU42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="BV42" s="49">
+      <c r="BV42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="BW42" s="49">
+      <c r="BW42" s="29">
         <f ca="1"/>
-        <v>152740</v>
-      </c>
-      <c r="BX42" s="49">
+        <v>102856</v>
+      </c>
+      <c r="BX42" s="29">
         <f ca="1"/>
-        <v>136366</v>
-      </c>
-      <c r="BY42" s="49">
+        <v>159254</v>
+      </c>
+      <c r="BY42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="BZ42" s="49">
+      <c r="BZ42" s="29">
         <f ca="1"/>
-        <v>336138</v>
-      </c>
-      <c r="CA42" s="49">
+        <v>373127</v>
+      </c>
+      <c r="CA42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="CB42" s="49">
+      <c r="CB42" s="29">
         <f ca="1"/>
-        <v>100388</v>
-      </c>
-      <c r="CC42" s="49">
+        <v>133449</v>
+      </c>
+      <c r="CC42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="CD42" s="49">
+      <c r="CD42" s="29">
         <f ca="1"/>
-        <v>373198</v>
-      </c>
-      <c r="CE42" s="49">
+        <v>0</v>
+      </c>
+      <c r="CE42" s="29">
         <f ca="1"/>
-        <v>194649</v>
-      </c>
-      <c r="CF42" s="49">
+        <v>305900</v>
+      </c>
+      <c r="CF42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="CG42" s="49">
+      <c r="CG42" s="29">
         <f ca="1"/>
-        <v>100133</v>
-      </c>
-      <c r="CH42" s="49">
+        <v>0</v>
+      </c>
+      <c r="CH42" s="29">
         <f ca="1"/>
-        <v>111610</v>
-      </c>
-      <c r="CI42" s="49">
+        <v>0</v>
+      </c>
+      <c r="CI42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="CJ42" s="49">
+      <c r="CJ42" s="29">
         <f ca="1"/>
-        <v>278242</v>
-      </c>
-      <c r="CK42" s="49">
+        <v>150409</v>
+      </c>
+      <c r="CK42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="CL42" s="49">
+      <c r="CL42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="CM42" s="49">
+      <c r="CM42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="CN42" s="49">
+      <c r="CN42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="CO42" s="49">
+      <c r="CO42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="CP42" s="49">
+      <c r="CP42" s="29">
         <f ca="1"/>
-        <v>179689</v>
-      </c>
-      <c r="CQ42" s="49">
+        <v>177797</v>
+      </c>
+      <c r="CQ42" s="29">
         <f ca="1"/>
-        <v>110115</v>
-      </c>
-      <c r="CR42" s="49">
+        <v>0</v>
+      </c>
+      <c r="CR42" s="29">
         <f ca="1"/>
-        <v>165386</v>
-      </c>
-      <c r="CS42" s="49">
+        <v>155897</v>
+      </c>
+      <c r="CS42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="CT42" s="49">
+      <c r="CT42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="CU42" s="49">
+      <c r="CU42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="CV42" s="49">
+      <c r="CV42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="CW42" s="49">
+      <c r="CW42" s="29">
         <f ca="1"/>
-        <v>138166</v>
-      </c>
-      <c r="CX42" s="49">
+        <v>0</v>
+      </c>
+      <c r="CX42" s="29">
         <f ca="1"/>
-        <v>171409</v>
-      </c>
-      <c r="CY42" s="49">
+        <v>0</v>
+      </c>
+      <c r="CY42" s="29">
         <f ca="1"/>
-        <v>142335</v>
-      </c>
-      <c r="CZ42" s="49">
+        <v>183287</v>
+      </c>
+      <c r="CZ42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="DA42" s="49">
+      <c r="DA42" s="29">
         <f ca="1"/>
-        <v>149587</v>
-      </c>
-      <c r="DB42" s="49">
+        <v>0</v>
+      </c>
+      <c r="DB42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="DC42" s="49">
+      <c r="DC42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="DD42" s="49">
+      <c r="DD42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="DE42" s="49">
+      <c r="DE42" s="29">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="DF42" s="49">
+      <c r="DF42" s="29">
         <f ca="1"/>
-        <v>246057</v>
+        <v>101395</v>
       </c>
     </row>
     <row r="43" spans="1:110" x14ac:dyDescent="0.3">
@@ -16141,7 +16287,8 @@
       <c r="DF182" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="A3:B3"/>
     <mergeCell ref="I8:N8"/>
     <mergeCell ref="B37:G37"/>
     <mergeCell ref="B38:G38"/>
@@ -16186,25 +16333,20 @@
       <formula1>$E$22:$DF$22</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="B38" r:id="rId1" xr:uid="{84322C72-FE3A-4232-AFB2-9DA3146E1E60}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DC12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="CR24" sqref="CR24"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -20195,29 +20337,26 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB032AE0-C04D-4D09-B0BF-943A8A88BBAC}">
-  <sheetPr>
-    <tabColor rgb="FFFFFF00"/>
-  </sheetPr>
-  <dimension ref="A1:DF121"/>
+  <dimension ref="A1:DG121"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="9"/>
-    <col min="2" max="2" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="9"/>
-    <col min="5" max="5" width="24.6640625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" style="9" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="9"/>
+    <col min="1" max="2" width="8.88671875" style="9"/>
+    <col min="3" max="3" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="9"/>
+    <col min="6" max="6" width="24.6640625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" style="9" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9"/>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -20236,17 +20375,20 @@
       <c r="P1" s="9"/>
       <c r="Q1" s="9"/>
       <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
     </row>
-    <row r="2" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
+    <row r="2" spans="1:19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="46" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
       <c r="D2" s="9"/>
-      <c r="E2" s="42" t="s">
-        <v>136</v>
-      </c>
-      <c r="F2" s="43"/>
-      <c r="G2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="G2" s="40"/>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
@@ -20258,21 +20400,22 @@
       <c r="P2" s="9"/>
       <c r="Q2" s="9"/>
       <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
     </row>
-    <row r="3" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="8" t="s">
-        <v>134</v>
-      </c>
+      <c r="E3" s="9"/>
       <c r="F3" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="G3" s="9"/>
+        <v>132</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>133</v>
+      </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -20284,20 +20427,21 @@
       <c r="P3" s="9"/>
       <c r="Q3" s="9"/>
       <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
     </row>
-    <row r="4" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
-      <c r="C4" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>77</v>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10" t="s">
+        <v>109</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="G4" s="9"/>
+        <v>79</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>60</v>
+      </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -20309,11 +20453,12 @@
       <c r="P4" s="9"/>
       <c r="Q4" s="9"/>
       <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
     </row>
-    <row r="5" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
-      <c r="D5" s="9"/>
+      <c r="C5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
@@ -20328,14 +20473,15 @@
       <c r="P5" s="9"/>
       <c r="Q5" s="9"/>
       <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
     </row>
-    <row r="6" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
-      <c r="C6" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="D6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
@@ -20350,17 +20496,18 @@
       <c r="P6" s="9"/>
       <c r="Q6" s="9"/>
       <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
     </row>
-    <row r="7" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="9"/>
+      <c r="C7" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C7" s="1" cm="1">
-        <f t="array" ref="C7">SUMPRODUCT((candidate_list=candidate)*vote_list)</f>
-        <v>1587537</v>
-      </c>
-      <c r="D7" s="9"/>
+      <c r="D7" s="1" cm="1">
+        <f t="array" ref="D7">SUMPRODUCT((candidate_list=candidate)*vote_list)</f>
+        <v>8109799</v>
+      </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
@@ -20375,18 +20522,19 @@
       <c r="P7" s="9"/>
       <c r="Q7" s="9"/>
       <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
     </row>
-    <row r="8" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
-      <c r="B8" s="2" t="str">
+      <c r="B8" s="9"/>
+      <c r="C8" s="2" t="str">
         <f>IF(city1="","None selected",city1)</f>
-        <v>Paris</v>
-      </c>
-      <c r="C8" s="1" cm="1">
-        <f t="array" ref="C8">SUMPRODUCT((candidate_list=candidate)*(city_list=city1)*vote_list)</f>
-        <v>80373</v>
-      </c>
-      <c r="D8" s="9"/>
+        <v>Polynésie française</v>
+      </c>
+      <c r="D8" s="1" cm="1">
+        <f t="array" ref="D8">SUMPRODUCT((candidate_list=candidate)*(city_list=city1)*vote_list)</f>
+        <v>11797</v>
+      </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
@@ -20401,18 +20549,19 @@
       <c r="P8" s="9"/>
       <c r="Q8" s="9"/>
       <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
     </row>
-    <row r="9" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
-      <c r="B9" s="2" t="str">
+      <c r="B9" s="9"/>
+      <c r="C9" s="2" t="str">
         <f>IF(city2="","None selected",city2)</f>
-        <v>Loire-Atlantique</v>
-      </c>
-      <c r="C9" s="1" cm="1">
-        <f t="array" ref="C9">SUMPRODUCT((candidate_list=candidate)*(city_list=city2)*vote_list)</f>
-        <v>60072</v>
-      </c>
-      <c r="D9" s="9"/>
+        <v>Lot-et-Garonne</v>
+      </c>
+      <c r="D9" s="1" cm="1">
+        <f t="array" ref="D9">SUMPRODUCT((candidate_list=candidate)*(city_list=city2)*vote_list)</f>
+        <v>50288</v>
+      </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
@@ -20427,8 +20576,9 @@
       <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
       <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
     </row>
-    <row r="10" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -20447,8 +20597,9 @@
       <c r="P10" s="9"/>
       <c r="Q10" s="9"/>
       <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
     </row>
-    <row r="11" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -20467,16 +20618,17 @@
       <c r="P11" s="9"/>
       <c r="Q11" s="9"/>
       <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
     </row>
-    <row r="12" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9"/>
-      <c r="B12" s="44" t="s">
-        <v>133</v>
-      </c>
-      <c r="C12" s="46" t="s">
-        <v>132</v>
-      </c>
-      <c r="D12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="41" t="s">
+        <v>131</v>
+      </c>
+      <c r="D12" s="43" t="s">
+        <v>130</v>
+      </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
@@ -20491,12 +20643,13 @@
       <c r="P12" s="9"/>
       <c r="Q12" s="9"/>
       <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
     </row>
-    <row r="13" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
-      <c r="B13" s="44"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="43"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
@@ -20511,12 +20664,13 @@
       <c r="P13" s="9"/>
       <c r="Q13" s="9"/>
       <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
     </row>
-    <row r="14" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
-      <c r="B14" s="45"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="43"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
@@ -20531,18 +20685,19 @@
       <c r="P14" s="9"/>
       <c r="Q14" s="9"/>
       <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
     </row>
-    <row r="15" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
-      <c r="B15" s="2" t="str" cm="1">
-        <f t="array" ref="B15">INDEX(city_list,1,MATCH(LARGE((candidate_list=candidate)*vote_list,1),_xlfn._xlws.FILTER((candidate_list=candidate)*vote_list,$D$31:$D$41&lt;&gt;0),0))</f>
-        <v>Paris</v>
-      </c>
-      <c r="C15" s="1" cm="1">
-        <f t="array" ref="C15">LARGE((candidate_list=candidate)*vote_list,1)</f>
-        <v>80373</v>
-      </c>
-      <c r="D15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="2" t="str" cm="1">
+        <f t="array" ref="C15">INDEX(city_list,1,MATCH(LARGE((candidate_list=candidate)*vote_list,1),_xlfn._xlws.FILTER((candidate_list=candidate)*vote_list,$E$31:$E$41&lt;&gt;0),0))</f>
+        <v>Nord</v>
+      </c>
+      <c r="D15" s="1" cm="1">
+        <f t="array" ref="D15">LARGE((candidate_list=candidate)*vote_list,1)</f>
+        <v>373127</v>
+      </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
@@ -20557,18 +20712,19 @@
       <c r="P15" s="9"/>
       <c r="Q15" s="9"/>
       <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
     </row>
-    <row r="16" spans="1:18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9"/>
-      <c r="B16" s="2" t="str" cm="1">
-        <f t="array" ref="B16">INDEX(city_list,1,MATCH(LARGE((candidate_list=candidate)*vote_list,2),_xlfn._xlws.FILTER((candidate_list=candidate)*vote_list,$D$31:$D$41&lt;&gt;0),0))</f>
-        <v>Loire-Atlantique</v>
-      </c>
-      <c r="C16" s="1" cm="1">
-        <f t="array" ref="C16">LARGE((candidate_list=candidate)*vote_list,2)</f>
-        <v>60072</v>
-      </c>
-      <c r="D16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="2" t="str" cm="1">
+        <f t="array" ref="C16">INDEX(city_list,1,MATCH(LARGE((candidate_list=candidate)*vote_list,2),_xlfn._xlws.FILTER((candidate_list=candidate)*vote_list,$E$31:$E$41&lt;&gt;0),0))</f>
+        <v>Pas-de-Calais</v>
+      </c>
+      <c r="D16" s="1" cm="1">
+        <f t="array" ref="D16">LARGE((candidate_list=candidate)*vote_list,2)</f>
+        <v>305900</v>
+      </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
@@ -20583,17 +20739,18 @@
       <c r="P16" s="9"/>
       <c r="Q16" s="9"/>
       <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
     </row>
-    <row r="17" spans="1:110" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="2" t="str" cm="1">
-        <f t="array" ref="B17">INDEX(city_list,1,MATCH(LARGE((candidate_list=candidate)*vote_list,3),_xlfn._xlws.FILTER((candidate_list=candidate)*vote_list,$D$31:$D$41&lt;&gt;0),0))</f>
-        <v>Rhône</v>
-      </c>
-      <c r="C17" s="1" cm="1">
-        <f t="array" ref="C17">LARGE((candidate_list=candidate)*vote_list,3)</f>
-        <v>51907</v>
-      </c>
-      <c r="D17" s="9"/>
+    <row r="17" spans="1:111" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="9"/>
+      <c r="C17" s="2" t="str" cm="1">
+        <f t="array" ref="C17">INDEX(city_list,1,MATCH(LARGE((candidate_list=candidate)*vote_list,3),_xlfn._xlws.FILTER((candidate_list=candidate)*vote_list,$E$31:$E$41&lt;&gt;0),0))</f>
+        <v>Bouches-du-Rhône</v>
+      </c>
+      <c r="D17" s="1" cm="1">
+        <f t="array" ref="D17">LARGE((candidate_list=candidate)*vote_list,3)</f>
+        <v>264754</v>
+      </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
@@ -20608,8 +20765,9 @@
       <c r="P17" s="9"/>
       <c r="Q17" s="9"/>
       <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
     </row>
-    <row r="18" spans="1:110" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:111" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -20628,8 +20786,9 @@
       <c r="P18" s="9"/>
       <c r="Q18" s="9"/>
       <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
     </row>
-    <row r="19" spans="1:110" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:111" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -20648,8 +20807,9 @@
       <c r="P19" s="9"/>
       <c r="Q19" s="9"/>
       <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
     </row>
-    <row r="20" spans="1:110" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:111" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -20668,8 +20828,9 @@
       <c r="P20" s="9"/>
       <c r="Q20" s="9"/>
       <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
     </row>
-    <row r="21" spans="1:110" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:111" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -20688,8 +20849,9 @@
       <c r="P21" s="9"/>
       <c r="Q21" s="9"/>
       <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
     </row>
-    <row r="22" spans="1:110" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:111" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -20708,8 +20870,9 @@
       <c r="P22" s="9"/>
       <c r="Q22" s="9"/>
       <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
     </row>
-    <row r="23" spans="1:110" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:111" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -20728,8 +20891,9 @@
       <c r="P23" s="9"/>
       <c r="Q23" s="9"/>
       <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
     </row>
-    <row r="24" spans="1:110" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:111" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -20748,8 +20912,9 @@
       <c r="P24" s="9"/>
       <c r="Q24" s="9"/>
       <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
     </row>
-    <row r="25" spans="1:110" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:111" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -20768,8 +20933,9 @@
       <c r="P25" s="9"/>
       <c r="Q25" s="9"/>
       <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
     </row>
-    <row r="26" spans="1:110" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:111" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -20788,8 +20954,9 @@
       <c r="P26" s="9"/>
       <c r="Q26" s="9"/>
       <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
     </row>
-    <row r="27" spans="1:110" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:111" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -20808,13 +20975,11 @@
       <c r="P27" s="9"/>
       <c r="Q27" s="9"/>
       <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
     </row>
-    <row r="31" spans="1:110" x14ac:dyDescent="0.3">
-      <c r="D31" s="15" cm="1">
-        <f t="array" ref="D31:DE41">(candidate_list=candidate)*vote_list</f>
-        <v>0</v>
-      </c>
-      <c r="E31" s="15">
+    <row r="31" spans="1:111" x14ac:dyDescent="0.3">
+      <c r="E31" s="15" cm="1">
+        <f t="array" ref="E31:DF41">(candidate_list=candidate)*vote_list</f>
         <v>0</v>
       </c>
       <c r="F31" s="15">
@@ -21129,12 +21294,12 @@
       <c r="DE31" s="15">
         <v>0</v>
       </c>
-      <c r="DF31" s="15"/>
+      <c r="DF31" s="15">
+        <v>0</v>
+      </c>
+      <c r="DG31" s="15"/>
     </row>
-    <row r="32" spans="1:110" x14ac:dyDescent="0.3">
-      <c r="D32" s="15">
-        <v>0</v>
-      </c>
+    <row r="32" spans="1:111" x14ac:dyDescent="0.3">
       <c r="E32" s="15">
         <v>0</v>
       </c>
@@ -21450,12 +21615,12 @@
       <c r="DE32" s="15">
         <v>0</v>
       </c>
-      <c r="DF32" s="15"/>
+      <c r="DF32" s="15">
+        <v>0</v>
+      </c>
+      <c r="DG32" s="15"/>
     </row>
-    <row r="33" spans="2:110" x14ac:dyDescent="0.3">
-      <c r="D33" s="15">
-        <v>0</v>
-      </c>
+    <row r="33" spans="3:111" x14ac:dyDescent="0.3">
       <c r="E33" s="15">
         <v>0</v>
       </c>
@@ -21771,12 +21936,12 @@
       <c r="DE33" s="15">
         <v>0</v>
       </c>
-      <c r="DF33" s="15"/>
+      <c r="DF33" s="15">
+        <v>0</v>
+      </c>
+      <c r="DG33" s="15"/>
     </row>
-    <row r="34" spans="2:110" x14ac:dyDescent="0.3">
-      <c r="D34" s="15">
-        <v>0</v>
-      </c>
+    <row r="34" spans="3:111" x14ac:dyDescent="0.3">
       <c r="E34" s="15">
         <v>0</v>
       </c>
@@ -22092,12 +22257,12 @@
       <c r="DE34" s="15">
         <v>0</v>
       </c>
-      <c r="DF34" s="15"/>
+      <c r="DF34" s="15">
+        <v>0</v>
+      </c>
+      <c r="DG34" s="15"/>
     </row>
-    <row r="35" spans="2:110" x14ac:dyDescent="0.3">
-      <c r="D35" s="15">
-        <v>0</v>
-      </c>
+    <row r="35" spans="3:111" x14ac:dyDescent="0.3">
       <c r="E35" s="15">
         <v>0</v>
       </c>
@@ -22413,12 +22578,12 @@
       <c r="DE35" s="15">
         <v>0</v>
       </c>
-      <c r="DF35" s="15"/>
+      <c r="DF35" s="15">
+        <v>0</v>
+      </c>
+      <c r="DG35" s="15"/>
     </row>
-    <row r="36" spans="2:110" x14ac:dyDescent="0.3">
-      <c r="D36" s="15">
-        <v>0</v>
-      </c>
+    <row r="36" spans="3:111" x14ac:dyDescent="0.3">
       <c r="E36" s="15">
         <v>0</v>
       </c>
@@ -22734,333 +22899,333 @@
       <c r="DE36" s="15">
         <v>0</v>
       </c>
-      <c r="DF36" s="15"/>
+      <c r="DF36" s="15">
+        <v>0</v>
+      </c>
+      <c r="DG36" s="15"/>
     </row>
-    <row r="37" spans="2:110" x14ac:dyDescent="0.3">
-      <c r="D37" s="15">
-        <v>0</v>
-      </c>
+    <row r="37" spans="3:111" x14ac:dyDescent="0.3">
       <c r="E37" s="15">
-        <v>0</v>
+        <v>86755</v>
       </c>
       <c r="F37" s="15">
-        <v>0</v>
+        <v>104677</v>
       </c>
       <c r="G37" s="15">
-        <v>0</v>
+        <v>50314</v>
       </c>
       <c r="H37" s="15">
-        <v>0</v>
+        <v>149218</v>
       </c>
       <c r="I37" s="15">
-        <v>0</v>
+        <v>26010</v>
       </c>
       <c r="J37" s="15">
-        <v>0</v>
+        <v>48227</v>
       </c>
       <c r="K37" s="15">
-        <v>0</v>
+        <v>49592</v>
       </c>
       <c r="L37" s="15">
-        <v>0</v>
+        <v>21958</v>
       </c>
       <c r="M37" s="15">
-        <v>0</v>
+        <v>49308</v>
       </c>
       <c r="N37" s="15">
-        <v>0</v>
+        <v>64027</v>
       </c>
       <c r="O37" s="15">
-        <v>0</v>
+        <v>34354</v>
       </c>
       <c r="P37" s="15">
-        <v>0</v>
+        <v>145869</v>
       </c>
       <c r="Q37" s="15">
-        <v>0</v>
+        <v>264754</v>
       </c>
       <c r="R37" s="15">
-        <v>0</v>
+        <v>91774</v>
       </c>
       <c r="S37" s="15">
-        <v>0</v>
+        <v>21570</v>
       </c>
       <c r="T37" s="15">
-        <v>0</v>
+        <v>50430</v>
       </c>
       <c r="U37" s="15">
-        <v>0</v>
+        <v>99791</v>
       </c>
       <c r="V37" s="15">
-        <v>0</v>
+        <v>44772</v>
       </c>
       <c r="W37" s="15">
-        <v>0</v>
+        <v>31658</v>
       </c>
       <c r="X37" s="15">
-        <v>0</v>
+        <v>20285</v>
       </c>
       <c r="Y37" s="15">
-        <v>0</v>
+        <v>16772</v>
       </c>
       <c r="Z37" s="15">
-        <v>0</v>
+        <v>69108</v>
       </c>
       <c r="AA37" s="15">
-        <v>0</v>
+        <v>79850</v>
       </c>
       <c r="AB37" s="15">
-        <v>0</v>
+        <v>47979</v>
       </c>
       <c r="AC37" s="15">
-        <v>0</v>
+        <v>63498</v>
       </c>
       <c r="AD37" s="15">
-        <v>0</v>
+        <v>66703</v>
       </c>
       <c r="AE37" s="15">
-        <v>0</v>
+        <v>70574</v>
       </c>
       <c r="AF37" s="15">
-        <v>0</v>
+        <v>105862</v>
       </c>
       <c r="AG37" s="15">
-        <v>0</v>
+        <v>102951</v>
       </c>
       <c r="AH37" s="15">
-        <v>0</v>
+        <v>61960</v>
       </c>
       <c r="AI37" s="15">
-        <v>0</v>
+        <v>100890</v>
       </c>
       <c r="AJ37" s="15">
-        <v>0</v>
+        <v>121478</v>
       </c>
       <c r="AK37" s="15">
-        <v>0</v>
+        <v>26013</v>
       </c>
       <c r="AL37" s="15">
-        <v>0</v>
+        <v>191542</v>
       </c>
       <c r="AM37" s="15">
-        <v>0</v>
+        <v>24204</v>
       </c>
       <c r="AN37" s="15">
-        <v>0</v>
+        <v>6334</v>
       </c>
       <c r="AO37" s="15">
-        <v>0</v>
+        <v>106930</v>
       </c>
       <c r="AP37" s="15">
-        <v>0</v>
+        <v>21999</v>
       </c>
       <c r="AQ37" s="15">
-        <v>0</v>
+        <v>133411</v>
       </c>
       <c r="AR37" s="15">
-        <v>0</v>
+        <v>38585</v>
       </c>
       <c r="AS37" s="15">
-        <v>0</v>
+        <v>34331</v>
       </c>
       <c r="AT37" s="15">
-        <v>0</v>
+        <v>87745</v>
       </c>
       <c r="AU37" s="15">
-        <v>0</v>
+        <v>46615</v>
       </c>
       <c r="AV37" s="15">
-        <v>0</v>
+        <v>45357</v>
       </c>
       <c r="AW37" s="15">
-        <v>0</v>
+        <v>19696</v>
       </c>
       <c r="AX37" s="15">
-        <v>0</v>
+        <v>29938</v>
       </c>
       <c r="AY37" s="15">
-        <v>0</v>
+        <v>64812</v>
       </c>
       <c r="AZ37" s="15">
-        <v>0</v>
+        <v>165729</v>
       </c>
       <c r="BA37" s="15">
-        <v>0</v>
+        <v>101797</v>
       </c>
       <c r="BB37" s="15">
-        <v>0</v>
+        <v>34514</v>
       </c>
       <c r="BC37" s="15">
-        <v>0</v>
+        <v>70553</v>
       </c>
       <c r="BD37" s="15">
-        <v>0</v>
+        <v>154889</v>
       </c>
       <c r="BE37" s="15">
-        <v>0</v>
+        <v>38177</v>
       </c>
       <c r="BF37" s="15">
-        <v>0</v>
+        <v>85770</v>
       </c>
       <c r="BG37" s="15">
-        <v>0</v>
+        <v>58646</v>
       </c>
       <c r="BH37" s="15">
-        <v>0</v>
+        <v>50212</v>
       </c>
       <c r="BI37" s="15">
-        <v>0</v>
+        <v>97846</v>
       </c>
       <c r="BJ37" s="15">
-        <v>0</v>
+        <v>135702</v>
       </c>
       <c r="BK37" s="15">
-        <v>0</v>
+        <v>85832</v>
       </c>
       <c r="BL37" s="15">
-        <v>0</v>
+        <v>21421</v>
       </c>
       <c r="BM37" s="15">
-        <v>0</v>
+        <v>50288</v>
       </c>
       <c r="BN37" s="15">
-        <v>0</v>
+        <v>10497</v>
       </c>
       <c r="BO37" s="15">
-        <v>0</v>
+        <v>89386</v>
       </c>
       <c r="BP37" s="15">
-        <v>0</v>
+        <v>69770</v>
       </c>
       <c r="BQ37" s="15">
-        <v>0</v>
+        <v>83756</v>
       </c>
       <c r="BR37" s="15">
-        <v>0</v>
+        <v>16495</v>
       </c>
       <c r="BS37" s="15">
-        <v>0</v>
+        <v>37376</v>
       </c>
       <c r="BT37" s="15">
-        <v>0</v>
+        <v>14958</v>
       </c>
       <c r="BU37" s="15">
-        <v>0</v>
+        <v>97282</v>
       </c>
       <c r="BV37" s="15">
-        <v>0</v>
+        <v>34582</v>
       </c>
       <c r="BW37" s="15">
-        <v>0</v>
+        <v>102856</v>
       </c>
       <c r="BX37" s="15">
-        <v>0</v>
+        <v>159254</v>
       </c>
       <c r="BY37" s="15">
-        <v>0</v>
+        <v>32838</v>
       </c>
       <c r="BZ37" s="15">
-        <v>0</v>
+        <v>373127</v>
       </c>
       <c r="CA37" s="15">
-        <v>0</v>
+        <v>13273</v>
       </c>
       <c r="CB37" s="15">
-        <v>0</v>
+        <v>133449</v>
       </c>
       <c r="CC37" s="15">
-        <v>0</v>
+        <v>41804</v>
       </c>
       <c r="CD37" s="15">
-        <v>0</v>
+        <v>58498</v>
       </c>
       <c r="CE37" s="15">
-        <v>0</v>
+        <v>305900</v>
       </c>
       <c r="CF37" s="15">
-        <v>0</v>
+        <v>11797</v>
       </c>
       <c r="CG37" s="15">
-        <v>0</v>
+        <v>78182</v>
       </c>
       <c r="CH37" s="15">
-        <v>0</v>
+        <v>69768</v>
       </c>
       <c r="CI37" s="15">
-        <v>0</v>
+        <v>87930</v>
       </c>
       <c r="CJ37" s="15">
-        <v>0</v>
+        <v>150409</v>
       </c>
       <c r="CK37" s="15">
-        <v>0</v>
+        <v>1445</v>
       </c>
       <c r="CL37" s="15">
-        <v>0</v>
+        <v>459</v>
       </c>
       <c r="CM37" s="15">
-        <v>0</v>
+        <v>82235</v>
       </c>
       <c r="CN37" s="15">
-        <v>0</v>
+        <v>56733</v>
       </c>
       <c r="CO37" s="15">
-        <v>0</v>
+        <v>81969</v>
       </c>
       <c r="CP37" s="15">
-        <v>0</v>
+        <v>177797</v>
       </c>
       <c r="CQ37" s="15">
-        <v>0</v>
+        <v>64541</v>
       </c>
       <c r="CR37" s="15">
-        <v>0</v>
+        <v>155897</v>
       </c>
       <c r="CS37" s="15">
-        <v>0</v>
+        <v>98208</v>
       </c>
       <c r="CT37" s="15">
-        <v>0</v>
+        <v>56543</v>
       </c>
       <c r="CU37" s="15">
-        <v>0</v>
+        <v>42182</v>
       </c>
       <c r="CV37" s="15">
-        <v>0</v>
+        <v>19061</v>
       </c>
       <c r="CW37" s="15">
-        <v>0</v>
+        <v>91081</v>
       </c>
       <c r="CX37" s="15">
-        <v>0</v>
+        <v>69599</v>
       </c>
       <c r="CY37" s="15">
-        <v>0</v>
+        <v>183287</v>
       </c>
       <c r="CZ37" s="15">
-        <v>0</v>
+        <v>89411</v>
       </c>
       <c r="DA37" s="15">
-        <v>0</v>
+        <v>97280</v>
       </c>
       <c r="DB37" s="15">
-        <v>0</v>
+        <v>54216</v>
       </c>
       <c r="DC37" s="15">
-        <v>0</v>
+        <v>65676</v>
       </c>
       <c r="DD37" s="15">
-        <v>0</v>
+        <v>579</v>
       </c>
       <c r="DE37" s="15">
-        <v>0</v>
-      </c>
-      <c r="DF37" s="15"/>
+        <v>55162</v>
+      </c>
+      <c r="DF37" s="15">
+        <v>101395</v>
+      </c>
+      <c r="DG37" s="15"/>
     </row>
-    <row r="38" spans="2:110" x14ac:dyDescent="0.3">
-      <c r="D38" s="15">
-        <v>0</v>
-      </c>
+    <row r="38" spans="3:111" x14ac:dyDescent="0.3">
       <c r="E38" s="15">
         <v>0</v>
       </c>
@@ -23376,333 +23541,333 @@
       <c r="DE38" s="15">
         <v>0</v>
       </c>
-      <c r="DF38" s="15"/>
+      <c r="DF38" s="15">
+        <v>0</v>
+      </c>
+      <c r="DG38" s="15"/>
     </row>
-    <row r="39" spans="2:110" x14ac:dyDescent="0.3">
-      <c r="D39" s="15">
-        <v>15843</v>
-      </c>
+    <row r="39" spans="3:111" x14ac:dyDescent="0.3">
       <c r="E39" s="15">
-        <v>7084</v>
+        <v>0</v>
       </c>
       <c r="F39" s="15">
-        <v>5982</v>
+        <v>0</v>
       </c>
       <c r="G39" s="15">
-        <v>23419</v>
+        <v>0</v>
       </c>
       <c r="H39" s="15">
-        <v>3957</v>
+        <v>0</v>
       </c>
       <c r="I39" s="15">
-        <v>3449</v>
+        <v>0</v>
       </c>
       <c r="J39" s="15">
-        <v>8544</v>
+        <v>0</v>
       </c>
       <c r="K39" s="15">
-        <v>3020</v>
+        <v>0</v>
       </c>
       <c r="L39" s="15">
-        <v>4619</v>
+        <v>0</v>
       </c>
       <c r="M39" s="15">
-        <v>6322</v>
+        <v>0</v>
       </c>
       <c r="N39" s="15">
-        <v>6746</v>
+        <v>0</v>
       </c>
       <c r="O39" s="15">
-        <v>28579</v>
+        <v>0</v>
       </c>
       <c r="P39" s="15">
-        <v>42109</v>
+        <v>0</v>
       </c>
       <c r="Q39" s="15">
-        <v>19641</v>
+        <v>0</v>
       </c>
       <c r="R39" s="15">
-        <v>2751</v>
+        <v>0</v>
       </c>
       <c r="S39" s="15">
-        <v>7557</v>
+        <v>0</v>
       </c>
       <c r="T39" s="15">
-        <v>19012</v>
+        <v>0</v>
       </c>
       <c r="U39" s="15">
-        <v>5028</v>
+        <v>0</v>
       </c>
       <c r="V39" s="15">
-        <v>5040</v>
+        <v>0</v>
       </c>
       <c r="W39" s="15">
-        <v>2281</v>
+        <v>0</v>
       </c>
       <c r="X39" s="15">
-        <v>1906</v>
+        <v>0</v>
       </c>
       <c r="Y39" s="15">
-        <v>13461</v>
+        <v>0</v>
       </c>
       <c r="Z39" s="15">
-        <v>19349</v>
+        <v>0</v>
       </c>
       <c r="AA39" s="15">
-        <v>10088</v>
+        <v>0</v>
       </c>
       <c r="AB39" s="15">
-        <v>8582</v>
+        <v>0</v>
       </c>
       <c r="AC39" s="15">
-        <v>13090</v>
+        <v>0</v>
       </c>
       <c r="AD39" s="15">
-        <v>14234</v>
+        <v>0</v>
       </c>
       <c r="AE39" s="15">
-        <v>29562</v>
+        <v>0</v>
       </c>
       <c r="AF39" s="15">
-        <v>11477</v>
+        <v>0</v>
       </c>
       <c r="AG39" s="15">
-        <v>7904</v>
+        <v>0</v>
       </c>
       <c r="AH39" s="15">
-        <v>33200</v>
+        <v>0</v>
       </c>
       <c r="AI39" s="15">
-        <v>14993</v>
+        <v>0</v>
       </c>
       <c r="AJ39" s="15">
-        <v>4089</v>
+        <v>0</v>
       </c>
       <c r="AK39" s="15">
-        <v>46677</v>
+        <v>0</v>
       </c>
       <c r="AL39" s="15">
-        <v>1927</v>
+        <v>0</v>
       </c>
       <c r="AM39" s="15">
-        <v>940</v>
+        <v>0</v>
       </c>
       <c r="AN39" s="15">
-        <v>18963</v>
+        <v>0</v>
       </c>
       <c r="AO39" s="15">
-        <v>2520</v>
+        <v>0</v>
       </c>
       <c r="AP39" s="15">
-        <v>42711</v>
+        <v>0</v>
       </c>
       <c r="AQ39" s="15">
-        <v>5796</v>
+        <v>0</v>
       </c>
       <c r="AR39" s="15">
-        <v>2580</v>
+        <v>0</v>
       </c>
       <c r="AS39" s="15">
-        <v>29948</v>
+        <v>0</v>
       </c>
       <c r="AT39" s="15">
-        <v>4291</v>
+        <v>0</v>
       </c>
       <c r="AU39" s="15">
-        <v>7877</v>
+        <v>0</v>
       </c>
       <c r="AV39" s="15">
-        <v>5013</v>
+        <v>0</v>
       </c>
       <c r="AW39" s="15">
-        <v>4870</v>
+        <v>0</v>
       </c>
       <c r="AX39" s="15">
-        <v>47103</v>
+        <v>0</v>
       </c>
       <c r="AY39" s="15">
-        <v>28057</v>
+        <v>0</v>
       </c>
       <c r="AZ39" s="15">
-        <v>42613</v>
+        <v>0</v>
       </c>
       <c r="BA39" s="15">
-        <v>3726</v>
+        <v>0</v>
       </c>
       <c r="BB39" s="15">
-        <v>16244</v>
+        <v>0</v>
       </c>
       <c r="BC39" s="15">
-        <v>40387</v>
+        <v>0</v>
       </c>
       <c r="BD39" s="15">
-        <v>6388</v>
+        <v>0</v>
       </c>
       <c r="BE39" s="15">
-        <v>7994</v>
+        <v>0</v>
       </c>
       <c r="BF39" s="15">
-        <v>8628</v>
+        <v>0</v>
       </c>
       <c r="BG39" s="15">
-        <v>7097</v>
+        <v>0</v>
       </c>
       <c r="BH39" s="15">
-        <v>16671</v>
+        <v>0</v>
       </c>
       <c r="BI39" s="15">
-        <v>60072</v>
+        <v>0</v>
       </c>
       <c r="BJ39" s="15">
-        <v>14401</v>
+        <v>0</v>
       </c>
       <c r="BK39" s="15">
-        <v>4603</v>
+        <v>0</v>
       </c>
       <c r="BL39" s="15">
-        <v>5685</v>
+        <v>0</v>
       </c>
       <c r="BM39" s="15">
-        <v>1736</v>
+        <v>0</v>
       </c>
       <c r="BN39" s="15">
-        <v>26614</v>
+        <v>0</v>
       </c>
       <c r="BO39" s="15">
-        <v>11873</v>
+        <v>0</v>
       </c>
       <c r="BP39" s="15">
-        <v>9561</v>
+        <v>0</v>
       </c>
       <c r="BQ39" s="15">
-        <v>1978</v>
+        <v>0</v>
       </c>
       <c r="BR39" s="15">
-        <v>7934</v>
+        <v>0</v>
       </c>
       <c r="BS39" s="15">
-        <v>295</v>
+        <v>0</v>
       </c>
       <c r="BT39" s="15">
-        <v>14593</v>
+        <v>0</v>
       </c>
       <c r="BU39" s="15">
-        <v>3130</v>
+        <v>0</v>
       </c>
       <c r="BV39" s="15">
-        <v>27036</v>
+        <v>0</v>
       </c>
       <c r="BW39" s="15">
-        <v>18931</v>
+        <v>0</v>
       </c>
       <c r="BX39" s="15">
-        <v>3552</v>
+        <v>0</v>
       </c>
       <c r="BY39" s="15">
-        <v>46962</v>
+        <v>0</v>
       </c>
       <c r="BZ39" s="15">
-        <v>2161</v>
+        <v>0</v>
       </c>
       <c r="CA39" s="15">
-        <v>13836</v>
+        <v>0</v>
       </c>
       <c r="CB39" s="15">
-        <v>5513</v>
+        <v>0</v>
       </c>
       <c r="CC39" s="15">
-        <v>80373</v>
+        <v>0</v>
       </c>
       <c r="CD39" s="15">
-        <v>19302</v>
+        <v>0</v>
       </c>
       <c r="CE39" s="15">
-        <v>2166</v>
+        <v>0</v>
       </c>
       <c r="CF39" s="15">
-        <v>17029</v>
+        <v>0</v>
       </c>
       <c r="CG39" s="15">
-        <v>19967</v>
+        <v>0</v>
       </c>
       <c r="CH39" s="15">
-        <v>8587</v>
+        <v>0</v>
       </c>
       <c r="CI39" s="15">
-        <v>51907</v>
+        <v>0</v>
       </c>
       <c r="CJ39" s="15">
-        <v>247</v>
+        <v>0</v>
       </c>
       <c r="CK39" s="15">
-        <v>116</v>
+        <v>0</v>
       </c>
       <c r="CL39" s="15">
-        <v>13541</v>
+        <v>0</v>
       </c>
       <c r="CM39" s="15">
-        <v>15642</v>
+        <v>0</v>
       </c>
       <c r="CN39" s="15">
-        <v>10730</v>
+        <v>0</v>
       </c>
       <c r="CO39" s="15">
-        <v>24784</v>
+        <v>0</v>
       </c>
       <c r="CP39" s="15">
-        <v>19352</v>
+        <v>0</v>
       </c>
       <c r="CQ39" s="15">
-        <v>26754</v>
+        <v>0</v>
       </c>
       <c r="CR39" s="15">
-        <v>8050</v>
+        <v>0</v>
       </c>
       <c r="CS39" s="15">
-        <v>8680</v>
+        <v>0</v>
       </c>
       <c r="CT39" s="15">
-        <v>4835</v>
+        <v>0</v>
       </c>
       <c r="CU39" s="15">
-        <v>2798</v>
+        <v>0</v>
       </c>
       <c r="CV39" s="15">
-        <v>20710</v>
+        <v>0</v>
       </c>
       <c r="CW39" s="15">
-        <v>31904</v>
+        <v>0</v>
       </c>
       <c r="CX39" s="15">
-        <v>21044</v>
+        <v>0</v>
       </c>
       <c r="CY39" s="15">
-        <v>12128</v>
+        <v>0</v>
       </c>
       <c r="CZ39" s="15">
-        <v>19731</v>
+        <v>0</v>
       </c>
       <c r="DA39" s="15">
-        <v>10727</v>
+        <v>0</v>
       </c>
       <c r="DB39" s="15">
-        <v>7569</v>
+        <v>0</v>
       </c>
       <c r="DC39" s="15">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="DD39" s="15">
-        <v>5917</v>
+        <v>0</v>
       </c>
       <c r="DE39" s="15">
-        <v>40470</v>
-      </c>
-      <c r="DF39" s="15"/>
+        <v>0</v>
+      </c>
+      <c r="DF39" s="15">
+        <v>0</v>
+      </c>
+      <c r="DG39" s="15"/>
     </row>
-    <row r="40" spans="2:110" x14ac:dyDescent="0.3">
-      <c r="D40" s="15">
-        <v>0</v>
-      </c>
+    <row r="40" spans="3:111" x14ac:dyDescent="0.3">
       <c r="E40" s="15">
         <v>0</v>
       </c>
@@ -24018,12 +24183,12 @@
       <c r="DE40" s="15">
         <v>0</v>
       </c>
-      <c r="DF40" s="15"/>
+      <c r="DF40" s="15">
+        <v>0</v>
+      </c>
+      <c r="DG40" s="15"/>
     </row>
-    <row r="41" spans="2:110" x14ac:dyDescent="0.3">
-      <c r="D41" s="15">
-        <v>0</v>
-      </c>
+    <row r="41" spans="3:111" x14ac:dyDescent="0.3">
       <c r="E41" s="15">
         <v>0</v>
       </c>
@@ -24339,37 +24504,41 @@
       <c r="DE41" s="15">
         <v>0</v>
       </c>
-      <c r="DF41" s="15"/>
+      <c r="DF41" s="15">
+        <v>0</v>
+      </c>
+      <c r="DG41" s="15"/>
     </row>
-    <row r="43" spans="2:110" x14ac:dyDescent="0.3">
-      <c r="B43" s="47"/>
-      <c r="C43" s="47"/>
-      <c r="D43" s="47"/>
-      <c r="E43" s="47"/>
-      <c r="F43" s="47"/>
-      <c r="G43" s="47"/>
+    <row r="43" spans="3:111" x14ac:dyDescent="0.3">
+      <c r="C43" s="44"/>
+      <c r="D43" s="44"/>
+      <c r="E43" s="44"/>
+      <c r="F43" s="44"/>
+      <c r="G43" s="44"/>
+      <c r="H43" s="44"/>
     </row>
-    <row r="44" spans="2:110" x14ac:dyDescent="0.3">
-      <c r="B44" s="48"/>
-      <c r="C44" s="48"/>
-      <c r="D44" s="48"/>
-      <c r="E44" s="48"/>
-      <c r="F44" s="48"/>
-      <c r="G44" s="48"/>
+    <row r="44" spans="3:111" x14ac:dyDescent="0.3">
+      <c r="C44" s="45"/>
+      <c r="D44" s="45"/>
+      <c r="E44" s="45"/>
+      <c r="F44" s="45"/>
+      <c r="G44" s="45"/>
+      <c r="H44" s="45"/>
     </row>
-    <row r="121" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D121" s="9" t="e" cm="1">
-        <f t="array" ref="D121">_xlfn._xlws.FILTER(IF((candidate_list=candidate)*vote_list,(candidate_list=candidate)*vote_list,""), IF((candidate_list=candidate)*vote_list,(candidate_list=candidate)*vote_list,"") &lt;&gt; "")</f>
+    <row r="121" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E121" s="9" t="e" cm="1">
+        <f t="array" ref="E121">_xlfn._xlws.FILTER(IF((candidate_list=candidate)*vote_list,(candidate_list=candidate)*vote_list,""), IF((candidate_list=candidate)*vote_list,(candidate_list=candidate)*vote_list,"") &lt;&gt; "")</f>
         <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="B12:B14"/>
+  <mergeCells count="6">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="F2:G2"/>
     <mergeCell ref="C12:C14"/>
-    <mergeCell ref="B43:G43"/>
-    <mergeCell ref="B44:G44"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="C43:H43"/>
+    <mergeCell ref="C44:H44"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -24382,13 +24551,13 @@
           <x14:formula1>
             <xm:f>Data!$A$2:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>C4</xm:sqref>
+          <xm:sqref>D4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{60FFF198-E6F7-4B10-9779-8C7DCE8A95DC}">
           <x14:formula1>
             <xm:f>Data!$B$1:$DC$1</xm:f>
           </x14:formula1>
-          <xm:sqref>E4:F4</xm:sqref>
+          <xm:sqref>F4:G4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>